<commit_message>
Add Vendors tab with 6 sample service partner companies for hospice management
</commit_message>
<xml_diff>
--- a/Dashboard Clone.xlsx
+++ b/Dashboard Clone.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Closed" sheetId="4" r:id="rId4"/>
     <sheet name="Oustanding" sheetId="5" r:id="rId5"/>
     <sheet name="Call Log" sheetId="6" r:id="rId6"/>
+    <sheet name="Vendors" sheetId="7" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -404,7 +405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -1490,7 +1491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -1823,7 +1824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -2057,7 +2058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -3098,7 +3099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -4148,7 +4149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -4475,4 +4476,305 @@
     <ignoredError numberStoredAsText="1" sqref="A1:I11"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Vendor ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Company Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Category</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Service Type</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Contact Person</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Address</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Website</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Notes</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Rating</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Last Contact</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Status</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>V001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Serenity Cremation Services</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Cremation</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Cremation &amp; Memorial</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Sarah Johnson</v>
+      </c>
+      <c r="F2" t="str">
+        <v>(555) 123-4567</v>
+      </c>
+      <c r="G2" t="str">
+        <v>sarah@serenitycremation.com</v>
+      </c>
+      <c r="H2" t="str">
+        <v>123 Peaceful Lane, Riverside, CA 92501</v>
+      </c>
+      <c r="I2" t="str">
+        <v>www.serenitycremation.com</v>
+      </c>
+      <c r="J2" t="str">
+        <v>Reliable service, good pricing</v>
+      </c>
+      <c r="K2" t="str">
+        <v>4.8</v>
+      </c>
+      <c r="L2" t="str">
+        <v>2024-01-15</v>
+      </c>
+      <c r="M2" t="str">
+        <v>Active</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>V002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Compassionate Care Pharmacies</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Pharmacy</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Hospice Medications</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Dr. Michael Chen</v>
+      </c>
+      <c r="F3" t="str">
+        <v>(555) 234-5678</v>
+      </c>
+      <c r="G3" t="str">
+        <v>mchen@compcarepharm.com</v>
+      </c>
+      <c r="H3" t="str">
+        <v>456 Medical Plaza, Riverside, CA 92503</v>
+      </c>
+      <c r="I3" t="str">
+        <v>www.compcarepharm.com</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Specializes in pain management meds</v>
+      </c>
+      <c r="K3" t="str">
+        <v>4.9</v>
+      </c>
+      <c r="L3" t="str">
+        <v>2024-01-20</v>
+      </c>
+      <c r="M3" t="str">
+        <v>Active</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>V003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Gentle Hands Doula Services</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Doula</v>
+      </c>
+      <c r="D4" t="str">
+        <v>End-of-Life Support</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Maria Rodriguez</v>
+      </c>
+      <c r="F4" t="str">
+        <v>(555) 345-6789</v>
+      </c>
+      <c r="G4" t="str">
+        <v>maria@gentlehands.com</v>
+      </c>
+      <c r="H4" t="str">
+        <v>789 Comfort Way, Riverside, CA 92505</v>
+      </c>
+      <c r="I4" t="str">
+        <v>www.gentlehands.com</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Excellent bedside manner, 24/7 availability</v>
+      </c>
+      <c r="K4" t="str">
+        <v>5.0</v>
+      </c>
+      <c r="L4" t="str">
+        <v>2024-01-18</v>
+      </c>
+      <c r="M4" t="str">
+        <v>Active</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>V004</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Eternal Rest Funeral Home</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Funeral Services</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Funeral &amp; Memorial</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Robert Williams</v>
+      </c>
+      <c r="F5" t="str">
+        <v>(555) 456-7890</v>
+      </c>
+      <c r="G5" t="str">
+        <v>rwilliams@eternalrest.com</v>
+      </c>
+      <c r="H5" t="str">
+        <v>321 Memorial Drive, Riverside, CA 92507</v>
+      </c>
+      <c r="I5" t="str">
+        <v>www.eternalrest.com</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Traditional services, family-owned</v>
+      </c>
+      <c r="K5" t="str">
+        <v>4.7</v>
+      </c>
+      <c r="L5" t="str">
+        <v>2024-01-12</v>
+      </c>
+      <c r="M5" t="str">
+        <v>Active</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>V005</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Hospice Equipment Supply Co.</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Medical Equipment</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Durable Medical Equipment</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Jennifer Davis</v>
+      </c>
+      <c r="F6" t="str">
+        <v>(555) 567-8901</v>
+      </c>
+      <c r="G6" t="str">
+        <v>jdavis@hospiceequipment.com</v>
+      </c>
+      <c r="H6" t="str">
+        <v>654 Medical Supply Blvd, Riverside, CA 92509</v>
+      </c>
+      <c r="I6" t="str">
+        <v>www.hospiceequipment.com</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Quick delivery, wide selection</v>
+      </c>
+      <c r="K6" t="str">
+        <v>4.6</v>
+      </c>
+      <c r="L6" t="str">
+        <v>2024-01-22</v>
+      </c>
+      <c r="M6" t="str">
+        <v>Active</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>V006</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Peaceful Transitions Counseling</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Counseling</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Grief &amp; Bereavement</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Dr. Lisa Thompson</v>
+      </c>
+      <c r="F7" t="str">
+        <v>(555) 678-9012</v>
+      </c>
+      <c r="G7" t="str">
+        <v>lthompson@peacefultransitions.com</v>
+      </c>
+      <c r="H7" t="str">
+        <v>987 Healing Circle, Riverside, CA 92511</v>
+      </c>
+      <c r="I7" t="str">
+        <v>www.peacefultransitions.com</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Licensed therapists, sliding scale fees</v>
+      </c>
+      <c r="K7" t="str">
+        <v>4.9</v>
+      </c>
+      <c r="L7" t="str">
+        <v>2024-01-16</v>
+      </c>
+      <c r="M7" t="str">
+        <v>Active</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:M7"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Team Chat functionality with XLSX storage and @mentions support
</commit_message>
<xml_diff>
--- a/Dashboard Clone.xlsx
+++ b/Dashboard Clone.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Oustanding" sheetId="5" r:id="rId5"/>
     <sheet name="Call Log" sheetId="6" r:id="rId6"/>
     <sheet name="Vendors" sheetId="7" r:id="rId7"/>
+    <sheet name="Chat" sheetId="8" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -4777,4 +4778,218 @@
     <ignoredError numberStoredAsText="1" sqref="A1:M7"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Timestamp</v>
+      </c>
+      <c r="B1" t="str">
+        <v>User</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Message</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Type</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Recipients</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Status</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>20241201143000</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Alyssa</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Hey team, where are we on the Johnson case?</v>
+      </c>
+      <c r="D2" t="str">
+        <v>question</v>
+      </c>
+      <c r="E2" t="str">
+        <v>all</v>
+      </c>
+      <c r="F2" t="str">
+        <v>active</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>20241201143100</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Dr. Moore</v>
+      </c>
+      <c r="C3" t="str">
+        <v>I just reviewed the medication list, all looks good</v>
+      </c>
+      <c r="D3" t="str">
+        <v>update</v>
+      </c>
+      <c r="E3" t="str">
+        <v>all</v>
+      </c>
+      <c r="F3" t="str">
+        <v>active</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>20241201143200</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Christa</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Family meeting scheduled for tomorrow at 2pm</v>
+      </c>
+      <c r="D4" t="str">
+        <v>info</v>
+      </c>
+      <c r="E4" t="str">
+        <v>all</v>
+      </c>
+      <c r="F4" t="str">
+        <v>active</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>20241201143300</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Amber</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Insurance approval came through!</v>
+      </c>
+      <c r="D5" t="str">
+        <v>good_news</v>
+      </c>
+      <c r="E5" t="str">
+        <v>all</v>
+      </c>
+      <c r="F5" t="str">
+        <v>active</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>20241201143400</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Alyssa</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Great work everyone!</v>
+      </c>
+      <c r="D6" t="str">
+        <v>comment</v>
+      </c>
+      <c r="E6" t="str">
+        <v>all</v>
+      </c>
+      <c r="F6" t="str">
+        <v>active</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>20241201143500</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Dr. Moore</v>
+      </c>
+      <c r="C7" t="str">
+        <v>@Christa - can you prep the meeting notes?</v>
+      </c>
+      <c r="D7" t="str">
+        <v>task</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Christa</v>
+      </c>
+      <c r="F7" t="str">
+        <v>active</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>20241201143600</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Christa</v>
+      </c>
+      <c r="C8" t="str">
+        <v>On it! Will have them ready by EOD</v>
+      </c>
+      <c r="D8" t="str">
+        <v>response</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Dr. Moore</v>
+      </c>
+      <c r="F8" t="str">
+        <v>active</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>20241201143700</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Amber</v>
+      </c>
+      <c r="C9" t="str">
+        <v>@Alyssa - need your input on the billing codes</v>
+      </c>
+      <c r="D9" t="str">
+        <v>question</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Alyssa</v>
+      </c>
+      <c r="F9" t="str">
+        <v>active</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>20241201143800</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Alyssa</v>
+      </c>
+      <c r="C10" t="str">
+        <v>I'll review and get back to you by 5pm</v>
+      </c>
+      <c r="D10" t="str">
+        <v>response</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Amber</v>
+      </c>
+      <c r="F10" t="str">
+        <v>active</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:F10"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement advanced chat system with DM/Group messages, user coding, and participant filtering
</commit_message>
<xml_diff>
--- a/Dashboard Clone.xlsx
+++ b/Dashboard Clone.xlsx
@@ -4782,7 +4782,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -4792,19 +4792,22 @@
         <v>Timestamp</v>
       </c>
       <c r="B1" t="str">
-        <v>User</v>
+        <v>Type</v>
       </c>
       <c r="C1" t="str">
+        <v>Participants</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Sender</v>
+      </c>
+      <c r="E1" t="str">
         <v>Message</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Type</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Recipients</v>
       </c>
       <c r="F1" t="str">
         <v>Status</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Tags</v>
       </c>
     </row>
     <row r="2">
@@ -4812,19 +4815,22 @@
         <v>20241201143000</v>
       </c>
       <c r="B2" t="str">
+        <v>GM</v>
+      </c>
+      <c r="C2" t="str">
+        <v>&lt;Alyssa&gt;&lt;Dr. Moore&gt;&lt;Christa&gt;&lt;Amber&gt;</v>
+      </c>
+      <c r="D2" t="str">
         <v>Alyssa</v>
       </c>
-      <c r="C2" t="str">
+      <c r="E2" t="str">
         <v>Hey team, where are we on the Johnson case?</v>
-      </c>
-      <c r="D2" t="str">
-        <v>question</v>
-      </c>
-      <c r="E2" t="str">
-        <v>all</v>
       </c>
       <c r="F2" t="str">
         <v>active</v>
+      </c>
+      <c r="G2" t="str">
+        <v>patient-update</v>
       </c>
     </row>
     <row r="3">
@@ -4832,19 +4838,22 @@
         <v>20241201143100</v>
       </c>
       <c r="B3" t="str">
+        <v>GM</v>
+      </c>
+      <c r="C3" t="str">
+        <v>&lt;Alyssa&gt;&lt;Dr. Moore&gt;&lt;Christa&gt;&lt;Amber&gt;</v>
+      </c>
+      <c r="D3" t="str">
         <v>Dr. Moore</v>
       </c>
-      <c r="C3" t="str">
+      <c r="E3" t="str">
         <v>I just reviewed the medication list, all looks good</v>
-      </c>
-      <c r="D3" t="str">
-        <v>update</v>
-      </c>
-      <c r="E3" t="str">
-        <v>all</v>
       </c>
       <c r="F3" t="str">
         <v>active</v>
+      </c>
+      <c r="G3" t="str">
+        <v>medical-review</v>
       </c>
     </row>
     <row r="4">
@@ -4852,19 +4861,22 @@
         <v>20241201143200</v>
       </c>
       <c r="B4" t="str">
+        <v>DM</v>
+      </c>
+      <c r="C4" t="str">
+        <v>&lt;Alyssa&gt;&lt;Christa&gt;</v>
+      </c>
+      <c r="D4" t="str">
         <v>Christa</v>
       </c>
-      <c r="C4" t="str">
+      <c r="E4" t="str">
         <v>Family meeting scheduled for tomorrow at 2pm</v>
-      </c>
-      <c r="D4" t="str">
-        <v>info</v>
-      </c>
-      <c r="E4" t="str">
-        <v>all</v>
       </c>
       <c r="F4" t="str">
         <v>active</v>
+      </c>
+      <c r="G4" t="str">
+        <v>meeting</v>
       </c>
     </row>
     <row r="5">
@@ -4872,19 +4884,22 @@
         <v>20241201143300</v>
       </c>
       <c r="B5" t="str">
-        <v>Amber</v>
+        <v>DM</v>
       </c>
       <c r="C5" t="str">
-        <v>Insurance approval came through!</v>
+        <v>&lt;Alyssa&gt;&lt;Amber&gt;</v>
       </c>
       <c r="D5" t="str">
-        <v>good_news</v>
+        <v>Alyssa</v>
       </c>
       <c r="E5" t="str">
-        <v>all</v>
+        <v>Hey Amber, can you prep the meeting notes?</v>
       </c>
       <c r="F5" t="str">
         <v>active</v>
+      </c>
+      <c r="G5" t="str">
+        <v>task</v>
       </c>
     </row>
     <row r="6">
@@ -4892,19 +4907,22 @@
         <v>20241201143400</v>
       </c>
       <c r="B6" t="str">
-        <v>Alyssa</v>
+        <v>GM</v>
       </c>
       <c r="C6" t="str">
-        <v>Great work everyone!</v>
+        <v>&lt;Alyssa&gt;&lt;Dr. Moore&gt;&lt;Christa&gt;&lt;Amber&gt;</v>
       </c>
       <c r="D6" t="str">
-        <v>comment</v>
+        <v>Amber</v>
       </c>
       <c r="E6" t="str">
-        <v>all</v>
+        <v>Welcome Amber! Please connect with Alyssa on this new project</v>
       </c>
       <c r="F6" t="str">
         <v>active</v>
+      </c>
+      <c r="G6" t="str">
+        <v>onboarding</v>
       </c>
     </row>
     <row r="7">
@@ -4912,19 +4930,22 @@
         <v>20241201143500</v>
       </c>
       <c r="B7" t="str">
+        <v>DM</v>
+      </c>
+      <c r="C7" t="str">
+        <v>&lt;Dr. Moore&gt;&lt;Christa&gt;</v>
+      </c>
+      <c r="D7" t="str">
         <v>Dr. Moore</v>
       </c>
-      <c r="C7" t="str">
-        <v>@Christa - can you prep the meeting notes?</v>
-      </c>
-      <c r="D7" t="str">
-        <v>task</v>
-      </c>
       <c r="E7" t="str">
-        <v>Christa</v>
+        <v>Christa, can you review the Johnson medication schedule?</v>
       </c>
       <c r="F7" t="str">
         <v>active</v>
+      </c>
+      <c r="G7" t="str">
+        <v>medical-task</v>
       </c>
     </row>
     <row r="8">
@@ -4932,19 +4953,22 @@
         <v>20241201143600</v>
       </c>
       <c r="B8" t="str">
-        <v>Christa</v>
+        <v>GM</v>
       </c>
       <c r="C8" t="str">
-        <v>On it! Will have them ready by EOD</v>
+        <v>&lt;Alyssa&gt;&lt;Dr. Moore&gt;&lt;Christa&gt;&lt;Amber&gt;</v>
       </c>
       <c r="D8" t="str">
-        <v>response</v>
+        <v>Alyssa</v>
       </c>
       <c r="E8" t="str">
-        <v>Dr. Moore</v>
+        <v>Insurance approval came through for the Smith family!</v>
       </c>
       <c r="F8" t="str">
         <v>active</v>
+      </c>
+      <c r="G8" t="str">
+        <v>good-news</v>
       </c>
     </row>
     <row r="9">
@@ -4952,19 +4976,22 @@
         <v>20241201143700</v>
       </c>
       <c r="B9" t="str">
-        <v>Amber</v>
+        <v>DM</v>
       </c>
       <c r="C9" t="str">
-        <v>@Alyssa - need your input on the billing codes</v>
+        <v>&lt;Alyssa&gt;&lt;Donnie&gt;</v>
       </c>
       <c r="D9" t="str">
-        <v>question</v>
+        <v>Alyssa</v>
       </c>
       <c r="E9" t="str">
-        <v>Alyssa</v>
+        <v>Hey Donnie, lets get Amber onboarded properly</v>
       </c>
       <c r="F9" t="str">
         <v>active</v>
+      </c>
+      <c r="G9" t="str">
+        <v>onboarding</v>
       </c>
     </row>
     <row r="10">
@@ -4972,24 +4999,119 @@
         <v>20241201143800</v>
       </c>
       <c r="B10" t="str">
-        <v>Alyssa</v>
+        <v>GM</v>
       </c>
       <c r="C10" t="str">
-        <v>I'll review and get back to you by 5pm</v>
+        <v>&lt;Alyssa&gt;&lt;Donnie&gt;&lt;Amber&gt;</v>
       </c>
       <c r="D10" t="str">
-        <v>response</v>
+        <v>Donnie</v>
       </c>
       <c r="E10" t="str">
-        <v>Amber</v>
+        <v>Welcome Amber! Please connect with Alyssa on this new project</v>
       </c>
       <c r="F10" t="str">
         <v>active</v>
       </c>
+      <c r="G10" t="str">
+        <v>welcome</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>20241201143900</v>
+      </c>
+      <c r="B11" t="str">
+        <v>NOTE</v>
+      </c>
+      <c r="C11" t="str">
+        <v>&lt;Alyssa&gt;</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Alyssa</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Patient timeline updated - family meeting scheduled</v>
+      </c>
+      <c r="F11" t="str">
+        <v>active</v>
+      </c>
+      <c r="G11" t="str">
+        <v>patient-timeline</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>20241201144000</v>
+      </c>
+      <c r="B12" t="str">
+        <v>NOTE</v>
+      </c>
+      <c r="C12" t="str">
+        <v>&lt;Dr. Moore&gt;</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Dr. Moore</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Medication review completed - no changes needed</v>
+      </c>
+      <c r="F12" t="str">
+        <v>active</v>
+      </c>
+      <c r="G12" t="str">
+        <v>medical-note</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>20241201144100</v>
+      </c>
+      <c r="B13" t="str">
+        <v>DM</v>
+      </c>
+      <c r="C13" t="str">
+        <v>&lt;Christa&gt;&lt;Amber&gt;</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Christa</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Amber, here are the key contacts for the Johnson case</v>
+      </c>
+      <c r="F13" t="str">
+        <v>active</v>
+      </c>
+      <c r="G13" t="str">
+        <v>contacts</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>20241201144200</v>
+      </c>
+      <c r="B14" t="str">
+        <v>GM</v>
+      </c>
+      <c r="C14" t="str">
+        <v>&lt;Alyssa&gt;&lt;Dr. Moore&gt;&lt;Christa&gt;&lt;Amber&gt;</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Amber</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Thanks everyone! Excited to be part of the team</v>
+      </c>
+      <c r="F14" t="str">
+        <v>active</v>
+      </c>
+      <c r="G14" t="str">
+        <v>introduction</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs(rules): tighten non-interactive defaults; cleanup test artifacts
</commit_message>
<xml_diff>
--- a/Dashboard Clone.xlsx
+++ b/Dashboard Clone.xlsx
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:AH11"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -429,78 +429,84 @@
         <v>Area</v>
       </c>
       <c r="G1" t="str">
+        <v>Phone Number</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="I1" t="str">
         <v>1st request</v>
       </c>
-      <c r="H1" t="str">
+      <c r="J1" t="str">
         <v>2nd request</v>
       </c>
-      <c r="I1" t="str">
+      <c r="K1" t="str">
         <v>CP Doctor</v>
       </c>
-      <c r="J1" t="str">
+      <c r="L1" t="str">
         <v>CP Completed</v>
       </c>
-      <c r="K1" t="str">
+      <c r="M1" t="str">
         <v>RXNT Info</v>
       </c>
-      <c r="L1" t="str">
+      <c r="N1" t="str">
         <v>WR</v>
       </c>
-      <c r="M1" t="str">
+      <c r="O1" t="str">
         <v>Hospice</v>
       </c>
-      <c r="N1" t="str">
+      <c r="P1" t="str">
         <v>Prescription Submit</v>
       </c>
-      <c r="O1" t="str">
-        <v/>
-      </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
+        <v/>
+      </c>
+      <c r="R1" t="str">
         <v>invoice amount</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="S1" t="str">
         <v>PAID</v>
       </c>
-      <c r="R1" t="str">
+      <c r="T1" t="str">
         <v>Check list</v>
       </c>
-      <c r="S1" t="str">
+      <c r="U1" t="str">
         <v>Ingestion Date</v>
       </c>
-      <c r="T1" t="str">
+      <c r="V1" t="str">
         <v>Ingestion Location</v>
       </c>
-      <c r="U1" t="str">
+      <c r="W1" t="str">
         <v>TTS (Minutes)</v>
       </c>
-      <c r="V1" t="str">
+      <c r="X1" t="str">
         <v>TTD (Minutes)</v>
       </c>
-      <c r="W1" t="str">
+      <c r="Y1" t="str">
         <v>Consent Received</v>
       </c>
-      <c r="X1" t="str">
+      <c r="Z1" t="str">
         <v>Medical Records</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="AA1" t="str">
         <v>Physician follow up form</v>
       </c>
-      <c r="Z1" t="str">
+      <c r="AB1" t="str">
         <v>EOLOA State</v>
       </c>
-      <c r="AA1" t="str">
+      <c r="AC1" t="str">
         <v>Death Certificate</v>
       </c>
-      <c r="AB1" t="str">
+      <c r="AD1" t="str">
         <v>All Recodrs in DRC</v>
       </c>
-      <c r="AC1" t="str">
-        <v/>
-      </c>
-      <c r="AD1" t="str">
+      <c r="AE1" t="str">
+        <v/>
+      </c>
+      <c r="AF1" t="str">
         <v>Riverside EOLOA</v>
       </c>
-      <c r="AE1" t="str">
+      <c r="AG1" t="str">
         <v>Referred From</v>
       </c>
     </row>
@@ -524,71 +530,71 @@
         <v>san diego</v>
       </c>
       <c r="G2" t="str">
+        <v>760-734-1214</v>
+      </c>
+      <c r="H2" t="str">
+        <v>adam255@hotmail.com</v>
+      </c>
+      <c r="I2" t="str">
         <v>45525</v>
       </c>
-      <c r="H2" t="str">
+      <c r="J2" t="str">
         <v>45527</v>
       </c>
-      <c r="I2" t="str">
+      <c r="K2" t="str">
         <v>Andzel</v>
       </c>
-      <c r="J2" t="str">
+      <c r="L2" t="str">
         <v>Gaja</v>
       </c>
-      <c r="K2" t="str">
+      <c r="M2" t="str">
         <v>45529</v>
       </c>
-      <c r="L2" t="str">
+      <c r="N2" t="str">
         <v>complete</v>
       </c>
-      <c r="M2" t="str">
+      <c r="O2" t="str">
         <v>45525</v>
       </c>
-      <c r="N2" t="str">
+      <c r="P2" t="str">
         <v>Radiant</v>
       </c>
-      <c r="O2" t="str">
+      <c r="Q2" t="str">
         <v>45530</v>
       </c>
-      <c r="P2" t="str">
-        <v/>
-      </c>
-      <c r="Q2" t="str">
+      <c r="R2" t="str">
+        <v/>
+      </c>
+      <c r="S2" t="str">
         <v>4200</v>
       </c>
-      <c r="R2" t="str">
-        <v>yes</v>
-      </c>
-      <c r="S2" t="str">
+      <c r="T2" t="str">
+        <v>yes</v>
+      </c>
+      <c r="U2" t="str">
         <v>complete</v>
       </c>
-      <c r="T2" t="str">
+      <c r="V2" t="str">
         <v>45536</v>
       </c>
-      <c r="U2" t="str">
+      <c r="W2" t="str">
         <v>residents</v>
       </c>
-      <c r="V2" t="str">
+      <c r="X2" t="str">
         <v>3</v>
       </c>
-      <c r="W2" t="str">
+      <c r="Y2" t="str">
         <v>64</v>
       </c>
-      <c r="X2" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y2" t="str">
-        <v>yes</v>
-      </c>
       <c r="Z2" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA2" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB2" t="str">
         <v>45545</v>
       </c>
-      <c r="AA2" t="str">
-        <v/>
-      </c>
-      <c r="AB2" t="str">
-        <v/>
-      </c>
       <c r="AC2" t="str">
         <v/>
       </c>
@@ -599,6 +605,12 @@
         <v/>
       </c>
       <c r="AF2" t="str">
+        <v/>
+      </c>
+      <c r="AG2" t="str">
+        <v/>
+      </c>
+      <c r="AH2" t="str">
         <v>Radiant Hospice</v>
       </c>
     </row>
@@ -622,14 +634,14 @@
         <v>La Jolla</v>
       </c>
       <c r="G3" t="str">
+        <v>951-218-4377</v>
+      </c>
+      <c r="H3" t="str">
+        <v>clare_burd@aol.com</v>
+      </c>
+      <c r="I3" t="str">
         <v>45720</v>
       </c>
-      <c r="H3" t="str">
-        <v/>
-      </c>
-      <c r="I3" t="str">
-        <v/>
-      </c>
       <c r="J3" t="str">
         <v/>
       </c>
@@ -694,6 +706,12 @@
         <v/>
       </c>
       <c r="AE3" t="str">
+        <v/>
+      </c>
+      <c r="AF3" t="str">
+        <v/>
+      </c>
+      <c r="AG3" t="str">
         <v/>
       </c>
     </row>
@@ -717,71 +735,71 @@
         <v>Encinitas</v>
       </c>
       <c r="G4" t="str">
+        <v>714-357-6734</v>
+      </c>
+      <c r="H4" t="str">
+        <v>emily_carter@yahoo.com</v>
+      </c>
+      <c r="I4" t="str">
         <v>45722</v>
       </c>
-      <c r="H4" t="str">
+      <c r="J4" t="str">
         <v>45724</v>
       </c>
-      <c r="I4" t="str">
+      <c r="K4" t="str">
         <v>Dr. Lisa Green</v>
       </c>
-      <c r="J4" t="str">
+      <c r="L4" t="str">
         <v>45726</v>
       </c>
-      <c r="K4" t="str">
+      <c r="M4" t="str">
         <v>complete</v>
       </c>
-      <c r="L4" t="str">
+      <c r="N4" t="str">
         <v>45723</v>
       </c>
-      <c r="M4" t="str">
-        <v>yes</v>
-      </c>
-      <c r="N4" t="str">
+      <c r="O4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="P4" t="str">
         <v>Serenity Hospice</v>
       </c>
-      <c r="O4" t="str">
+      <c r="Q4" t="str">
         <v>45727</v>
       </c>
-      <c r="P4" t="str">
-        <v/>
-      </c>
-      <c r="Q4" t="str">
+      <c r="R4" t="str">
+        <v/>
+      </c>
+      <c r="S4" t="str">
         <v>3500</v>
       </c>
-      <c r="R4" t="str">
-        <v>yes</v>
-      </c>
-      <c r="S4" t="str">
+      <c r="T4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="U4" t="str">
         <v>complete</v>
       </c>
-      <c r="T4" t="str">
+      <c r="V4" t="str">
         <v>45730</v>
       </c>
-      <c r="U4" t="str">
+      <c r="W4" t="str">
         <v>private home</v>
       </c>
-      <c r="V4" t="str">
+      <c r="X4" t="str">
         <v>5</v>
       </c>
-      <c r="W4" t="str">
+      <c r="Y4" t="str">
         <v>45</v>
       </c>
-      <c r="X4" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y4" t="str">
-        <v>yes</v>
-      </c>
       <c r="Z4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB4" t="str">
         <v>45735</v>
       </c>
-      <c r="AA4" t="str">
-        <v/>
-      </c>
-      <c r="AB4" t="str">
-        <v/>
-      </c>
       <c r="AC4" t="str">
         <v/>
       </c>
@@ -792,6 +810,12 @@
         <v/>
       </c>
       <c r="AF4" t="str">
+        <v/>
+      </c>
+      <c r="AG4" t="str">
+        <v/>
+      </c>
+      <c r="AH4" t="str">
         <v>Serenity Hospice</v>
       </c>
     </row>
@@ -815,71 +839,71 @@
         <v>San Diego</v>
       </c>
       <c r="G5" t="str">
+        <v>714-700-7058</v>
+      </c>
+      <c r="H5" t="str">
+        <v>frank.davis@hotmail.com</v>
+      </c>
+      <c r="I5" t="str">
         <v>45727</v>
       </c>
-      <c r="H5" t="str">
+      <c r="J5" t="str">
         <v>45729</v>
       </c>
-      <c r="I5" t="str">
+      <c r="K5" t="str">
         <v>Dr. Mark Hale</v>
       </c>
-      <c r="J5" t="str">
+      <c r="L5" t="str">
         <v>45731</v>
       </c>
-      <c r="K5" t="str">
+      <c r="M5" t="str">
         <v>pending</v>
       </c>
-      <c r="L5" t="str">
+      <c r="N5" t="str">
         <v>45728</v>
       </c>
-      <c r="M5" t="str">
+      <c r="O5" t="str">
         <v>no</v>
       </c>
-      <c r="N5" t="str">
+      <c r="P5" t="str">
         <v>Radiant</v>
       </c>
-      <c r="O5" t="str">
+      <c r="Q5" t="str">
         <v>45732</v>
       </c>
-      <c r="P5" t="str">
-        <v/>
-      </c>
-      <c r="Q5" t="str">
+      <c r="R5" t="str">
+        <v/>
+      </c>
+      <c r="S5" t="str">
         <v>2800</v>
       </c>
-      <c r="R5" t="str">
+      <c r="T5" t="str">
         <v>no</v>
       </c>
-      <c r="S5" t="str">
+      <c r="U5" t="str">
         <v>in progress</v>
       </c>
-      <c r="T5" t="str">
+      <c r="V5" t="str">
         <v>45735</v>
       </c>
-      <c r="U5" t="str">
+      <c r="W5" t="str">
         <v>assisted living</v>
       </c>
-      <c r="V5" t="str">
+      <c r="X5" t="str">
         <v>10</v>
       </c>
-      <c r="W5" t="str">
+      <c r="Y5" t="str">
         <v>120</v>
       </c>
-      <c r="X5" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y5" t="str">
+      <c r="Z5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA5" t="str">
         <v>no</v>
       </c>
-      <c r="Z5" t="str">
+      <c r="AB5" t="str">
         <v>45740</v>
       </c>
-      <c r="AA5" t="str">
-        <v/>
-      </c>
-      <c r="AB5" t="str">
-        <v/>
-      </c>
       <c r="AC5" t="str">
         <v/>
       </c>
@@ -890,6 +914,12 @@
         <v/>
       </c>
       <c r="AF5" t="str">
+        <v/>
+      </c>
+      <c r="AG5" t="str">
+        <v/>
+      </c>
+      <c r="AH5" t="str">
         <v>Radiant Hospice</v>
       </c>
     </row>
@@ -913,71 +943,71 @@
         <v>La Jolla</v>
       </c>
       <c r="G6" t="str">
+        <v>714-500-4286</v>
+      </c>
+      <c r="H6" t="str">
+        <v>grace_evans@hotmail.com</v>
+      </c>
+      <c r="I6" t="str">
         <v>45732</v>
       </c>
-      <c r="H6" t="str">
+      <c r="J6" t="str">
         <v>45734</v>
       </c>
-      <c r="I6" t="str">
+      <c r="K6" t="str">
         <v>Dr. Nina Ford</v>
       </c>
-      <c r="J6" t="str">
+      <c r="L6" t="str">
         <v>45736</v>
       </c>
-      <c r="K6" t="str">
+      <c r="M6" t="str">
         <v>complete</v>
       </c>
-      <c r="L6" t="str">
+      <c r="N6" t="str">
         <v>45733</v>
       </c>
-      <c r="M6" t="str">
-        <v>yes</v>
-      </c>
-      <c r="N6" t="str">
+      <c r="O6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="P6" t="str">
         <v>Harmony Care</v>
       </c>
-      <c r="O6" t="str">
+      <c r="Q6" t="str">
         <v>45737</v>
       </c>
-      <c r="P6" t="str">
-        <v/>
-      </c>
-      <c r="Q6" t="str">
+      <c r="R6" t="str">
+        <v/>
+      </c>
+      <c r="S6" t="str">
         <v>4100</v>
       </c>
-      <c r="R6" t="str">
-        <v>yes</v>
-      </c>
-      <c r="S6" t="str">
+      <c r="T6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="U6" t="str">
         <v>complete</v>
       </c>
-      <c r="T6" t="str">
+      <c r="V6" t="str">
         <v>45740</v>
       </c>
-      <c r="U6" t="str">
+      <c r="W6" t="str">
         <v>residents</v>
       </c>
-      <c r="V6" t="str">
+      <c r="X6" t="str">
         <v>2</v>
       </c>
-      <c r="W6" t="str">
+      <c r="Y6" t="str">
         <v>30</v>
       </c>
-      <c r="X6" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y6" t="str">
-        <v>yes</v>
-      </c>
       <c r="Z6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB6" t="str">
         <v>45745</v>
       </c>
-      <c r="AA6" t="str">
-        <v/>
-      </c>
-      <c r="AB6" t="str">
-        <v/>
-      </c>
       <c r="AC6" t="str">
         <v/>
       </c>
@@ -988,6 +1018,12 @@
         <v/>
       </c>
       <c r="AF6" t="str">
+        <v/>
+      </c>
+      <c r="AG6" t="str">
+        <v/>
+      </c>
+      <c r="AH6" t="str">
         <v>Harmony Care</v>
       </c>
     </row>
@@ -1011,71 +1047,71 @@
         <v>Oceanside</v>
       </c>
       <c r="G7" t="str">
+        <v>323-720-5970</v>
+      </c>
+      <c r="H7" t="str">
+        <v>henry_foster@yahoo.com</v>
+      </c>
+      <c r="I7" t="str">
         <v>45737</v>
       </c>
-      <c r="H7" t="str">
+      <c r="J7" t="str">
         <v>45739</v>
       </c>
-      <c r="I7" t="str">
+      <c r="K7" t="str">
         <v>Dr. Owen Gray</v>
       </c>
-      <c r="J7" t="str">
+      <c r="L7" t="str">
         <v>45741</v>
       </c>
-      <c r="K7" t="str">
+      <c r="M7" t="str">
         <v>complete</v>
       </c>
-      <c r="L7" t="str">
+      <c r="N7" t="str">
         <v>45738</v>
       </c>
-      <c r="M7" t="str">
+      <c r="O7" t="str">
         <v>no</v>
       </c>
-      <c r="N7" t="str">
+      <c r="P7" t="str">
         <v>Coastal Hospice</v>
       </c>
-      <c r="O7" t="str">
+      <c r="Q7" t="str">
         <v>45742</v>
       </c>
-      <c r="P7" t="str">
-        <v/>
-      </c>
-      <c r="Q7" t="str">
+      <c r="R7" t="str">
+        <v/>
+      </c>
+      <c r="S7" t="str">
         <v>3200</v>
       </c>
-      <c r="R7" t="str">
-        <v>yes</v>
-      </c>
-      <c r="S7" t="str">
+      <c r="T7" t="str">
+        <v>yes</v>
+      </c>
+      <c r="U7" t="str">
         <v>complete</v>
       </c>
-      <c r="T7" t="str">
+      <c r="V7" t="str">
         <v>45745</v>
       </c>
-      <c r="U7" t="str">
+      <c r="W7" t="str">
         <v>private home</v>
       </c>
-      <c r="V7" t="str">
+      <c r="X7" t="str">
         <v>4</v>
       </c>
-      <c r="W7" t="str">
+      <c r="Y7" t="str">
         <v>60</v>
       </c>
-      <c r="X7" t="str">
+      <c r="Z7" t="str">
         <v>no</v>
       </c>
-      <c r="Y7" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Z7" t="str">
+      <c r="AA7" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB7" t="str">
         <v>45750</v>
       </c>
-      <c r="AA7" t="str">
-        <v/>
-      </c>
-      <c r="AB7" t="str">
-        <v/>
-      </c>
       <c r="AC7" t="str">
         <v/>
       </c>
@@ -1086,6 +1122,12 @@
         <v/>
       </c>
       <c r="AF7" t="str">
+        <v/>
+      </c>
+      <c r="AG7" t="str">
+        <v/>
+      </c>
+      <c r="AH7" t="str">
         <v>Coastal Hospice</v>
       </c>
     </row>
@@ -1109,71 +1151,71 @@
         <v>Carlsbad</v>
       </c>
       <c r="G8" t="str">
+        <v>760-570-2681</v>
+      </c>
+      <c r="H8" t="str">
+        <v>igomez@outlook.com</v>
+      </c>
+      <c r="I8" t="str">
         <v>45742</v>
       </c>
-      <c r="H8" t="str">
+      <c r="J8" t="str">
         <v>45744</v>
       </c>
-      <c r="I8" t="str">
+      <c r="K8" t="str">
         <v>Dr. Paula Hunt</v>
       </c>
-      <c r="J8" t="str">
+      <c r="L8" t="str">
         <v>45746</v>
       </c>
-      <c r="K8" t="str">
+      <c r="M8" t="str">
         <v>pending</v>
       </c>
-      <c r="L8" t="str">
+      <c r="N8" t="str">
         <v>45743</v>
       </c>
-      <c r="M8" t="str">
-        <v>yes</v>
-      </c>
-      <c r="N8" t="str">
+      <c r="O8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="P8" t="str">
         <v>Sunrise Hospice</v>
       </c>
-      <c r="O8" t="str">
+      <c r="Q8" t="str">
         <v>45747</v>
       </c>
-      <c r="P8" t="str">
-        <v/>
-      </c>
-      <c r="Q8" t="str">
+      <c r="R8" t="str">
+        <v/>
+      </c>
+      <c r="S8" t="str">
         <v>3900</v>
       </c>
-      <c r="R8" t="str">
+      <c r="T8" t="str">
         <v>no</v>
       </c>
-      <c r="S8" t="str">
+      <c r="U8" t="str">
         <v>in progress</v>
       </c>
-      <c r="T8" t="str">
+      <c r="V8" t="str">
         <v>45750</v>
       </c>
-      <c r="U8" t="str">
+      <c r="W8" t="str">
         <v>acute care hospital</v>
       </c>
-      <c r="V8" t="str">
+      <c r="X8" t="str">
         <v>15</v>
       </c>
-      <c r="W8" t="str">
+      <c r="Y8" t="str">
         <v>180</v>
       </c>
-      <c r="X8" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y8" t="str">
-        <v>yes</v>
-      </c>
       <c r="Z8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB8" t="str">
         <v>45755</v>
       </c>
-      <c r="AA8" t="str">
-        <v/>
-      </c>
-      <c r="AB8" t="str">
-        <v/>
-      </c>
       <c r="AC8" t="str">
         <v/>
       </c>
@@ -1184,6 +1226,12 @@
         <v/>
       </c>
       <c r="AF8" t="str">
+        <v/>
+      </c>
+      <c r="AG8" t="str">
+        <v/>
+      </c>
+      <c r="AH8" t="str">
         <v>Sunrise Hospice</v>
       </c>
     </row>
@@ -1207,71 +1255,71 @@
         <v>Del Mar</v>
       </c>
       <c r="G9" t="str">
+        <v>323-618-5577</v>
+      </c>
+      <c r="H9" t="str">
+        <v>jackharris@yahoo.com</v>
+      </c>
+      <c r="I9" t="str">
         <v>45747</v>
       </c>
-      <c r="H9" t="str">
+      <c r="J9" t="str">
         <v>45749</v>
       </c>
-      <c r="I9" t="str">
+      <c r="K9" t="str">
         <v>Dr. Quentin Ives</v>
       </c>
-      <c r="J9" t="str">
+      <c r="L9" t="str">
         <v>45751</v>
       </c>
-      <c r="K9" t="str">
+      <c r="M9" t="str">
         <v>complete</v>
       </c>
-      <c r="L9" t="str">
+      <c r="N9" t="str">
         <v>45748</v>
       </c>
-      <c r="M9" t="str">
+      <c r="O9" t="str">
         <v>no</v>
       </c>
-      <c r="N9" t="str">
+      <c r="P9" t="str">
         <v>Eternal Peace</v>
       </c>
-      <c r="O9" t="str">
+      <c r="Q9" t="str">
         <v>45752</v>
       </c>
-      <c r="P9" t="str">
-        <v/>
-      </c>
-      <c r="Q9" t="str">
+      <c r="R9" t="str">
+        <v/>
+      </c>
+      <c r="S9" t="str">
         <v>2900</v>
       </c>
-      <c r="R9" t="str">
-        <v>yes</v>
-      </c>
-      <c r="S9" t="str">
+      <c r="T9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="U9" t="str">
         <v>complete</v>
       </c>
-      <c r="T9" t="str">
+      <c r="V9" t="str">
         <v>45755</v>
       </c>
-      <c r="U9" t="str">
+      <c r="W9" t="str">
         <v>in-patient hospice</v>
       </c>
-      <c r="V9" t="str">
+      <c r="X9" t="str">
         <v>3</v>
       </c>
-      <c r="W9" t="str">
+      <c r="Y9" t="str">
         <v>90</v>
       </c>
-      <c r="X9" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y9" t="str">
+      <c r="Z9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA9" t="str">
         <v>no</v>
       </c>
-      <c r="Z9" t="str">
+      <c r="AB9" t="str">
         <v>45760</v>
       </c>
-      <c r="AA9" t="str">
-        <v/>
-      </c>
-      <c r="AB9" t="str">
-        <v/>
-      </c>
       <c r="AC9" t="str">
         <v/>
       </c>
@@ -1282,6 +1330,12 @@
         <v/>
       </c>
       <c r="AF9" t="str">
+        <v/>
+      </c>
+      <c r="AG9" t="str">
+        <v/>
+      </c>
+      <c r="AH9" t="str">
         <v>Eternal Peace</v>
       </c>
     </row>
@@ -1305,71 +1359,71 @@
         <v>Vista</v>
       </c>
       <c r="G10" t="str">
+        <v>951-989-9017</v>
+      </c>
+      <c r="H10" t="str">
+        <v>karen_ingram@gmail.com</v>
+      </c>
+      <c r="I10" t="str">
         <v>45752</v>
       </c>
-      <c r="H10" t="str">
+      <c r="J10" t="str">
         <v>45754</v>
       </c>
-      <c r="I10" t="str">
+      <c r="K10" t="str">
         <v>Dr. Rachel James</v>
       </c>
-      <c r="J10" t="str">
+      <c r="L10" t="str">
         <v>45756</v>
       </c>
-      <c r="K10" t="str">
+      <c r="M10" t="str">
         <v>complete</v>
       </c>
-      <c r="L10" t="str">
+      <c r="N10" t="str">
         <v>45753</v>
       </c>
-      <c r="M10" t="str">
-        <v>yes</v>
-      </c>
-      <c r="N10" t="str">
+      <c r="O10" t="str">
+        <v>yes</v>
+      </c>
+      <c r="P10" t="str">
         <v>Tranquil Care</v>
       </c>
-      <c r="O10" t="str">
+      <c r="Q10" t="str">
         <v>45757</v>
       </c>
-      <c r="P10" t="str">
-        <v/>
-      </c>
-      <c r="Q10" t="str">
+      <c r="R10" t="str">
+        <v/>
+      </c>
+      <c r="S10" t="str">
         <v>4500</v>
       </c>
-      <c r="R10" t="str">
-        <v>yes</v>
-      </c>
-      <c r="S10" t="str">
+      <c r="T10" t="str">
+        <v>yes</v>
+      </c>
+      <c r="U10" t="str">
         <v>complete</v>
       </c>
-      <c r="T10" t="str">
+      <c r="V10" t="str">
         <v>45760</v>
       </c>
-      <c r="U10" t="str">
+      <c r="W10" t="str">
         <v>other</v>
       </c>
-      <c r="V10" t="str">
+      <c r="X10" t="str">
         <v>1</v>
       </c>
-      <c r="W10" t="str">
+      <c r="Y10" t="str">
         <v>20</v>
       </c>
-      <c r="X10" t="str">
+      <c r="Z10" t="str">
         <v>no</v>
       </c>
-      <c r="Y10" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Z10" t="str">
+      <c r="AA10" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB10" t="str">
         <v>45765</v>
       </c>
-      <c r="AA10" t="str">
-        <v/>
-      </c>
-      <c r="AB10" t="str">
-        <v/>
-      </c>
       <c r="AC10" t="str">
         <v/>
       </c>
@@ -1380,6 +1434,12 @@
         <v/>
       </c>
       <c r="AF10" t="str">
+        <v/>
+      </c>
+      <c r="AG10" t="str">
+        <v/>
+      </c>
+      <c r="AH10" t="str">
         <v>Tranquil Care</v>
       </c>
     </row>
@@ -1403,71 +1463,71 @@
         <v>Escondido</v>
       </c>
       <c r="G11" t="str">
+        <v>213-230-2901</v>
+      </c>
+      <c r="H11" t="str">
+        <v>ljackson@hotmail.com</v>
+      </c>
+      <c r="I11" t="str">
         <v>45757</v>
       </c>
-      <c r="H11" t="str">
+      <c r="J11" t="str">
         <v>45759</v>
       </c>
-      <c r="I11" t="str">
+      <c r="K11" t="str">
         <v>Dr. Sam Kline</v>
       </c>
-      <c r="J11" t="str">
+      <c r="L11" t="str">
         <v>45761</v>
       </c>
-      <c r="K11" t="str">
+      <c r="M11" t="str">
         <v>pending</v>
       </c>
-      <c r="L11" t="str">
+      <c r="N11" t="str">
         <v>45758</v>
       </c>
-      <c r="M11" t="str">
+      <c r="O11" t="str">
         <v>no</v>
       </c>
-      <c r="N11" t="str">
+      <c r="P11" t="str">
         <v>Peaceful End</v>
       </c>
-      <c r="O11" t="str">
+      <c r="Q11" t="str">
         <v>45762</v>
       </c>
-      <c r="P11" t="str">
-        <v/>
-      </c>
-      <c r="Q11" t="str">
+      <c r="R11" t="str">
+        <v/>
+      </c>
+      <c r="S11" t="str">
         <v>3100</v>
       </c>
-      <c r="R11" t="str">
+      <c r="T11" t="str">
         <v>no</v>
       </c>
-      <c r="S11" t="str">
+      <c r="U11" t="str">
         <v>in progress</v>
       </c>
-      <c r="T11" t="str">
+      <c r="V11" t="str">
         <v>45765</v>
       </c>
-      <c r="U11" t="str">
+      <c r="W11" t="str">
         <v>private home</v>
       </c>
-      <c r="V11" t="str">
+      <c r="X11" t="str">
         <v>6</v>
       </c>
-      <c r="W11" t="str">
+      <c r="Y11" t="str">
         <v>75</v>
       </c>
-      <c r="X11" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y11" t="str">
-        <v>yes</v>
-      </c>
       <c r="Z11" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA11" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB11" t="str">
         <v>45770</v>
       </c>
-      <c r="AA11" t="str">
-        <v/>
-      </c>
-      <c r="AB11" t="str">
-        <v/>
-      </c>
       <c r="AC11" t="str">
         <v/>
       </c>
@@ -1478,12 +1538,18 @@
         <v/>
       </c>
       <c r="AF11" t="str">
+        <v/>
+      </c>
+      <c r="AG11" t="str">
+        <v/>
+      </c>
+      <c r="AH11" t="str">
         <v>Peaceful End</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AF11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AH11"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3098,7 +3164,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE11"/>
+  <dimension ref="A1:AG11"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -3120,71 +3186,71 @@
         <v>Area</v>
       </c>
       <c r="F1" t="str">
+        <v>Phone Number</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="H1" t="str">
         <v>1st request</v>
       </c>
-      <c r="G1" t="str">
+      <c r="I1" t="str">
         <v>2nd request</v>
       </c>
-      <c r="H1" t="str">
+      <c r="J1" t="str">
         <v>CP Doctor</v>
       </c>
-      <c r="I1" t="str">
+      <c r="K1" t="str">
         <v>CP Completed</v>
       </c>
-      <c r="J1" t="str">
+      <c r="L1" t="str">
         <v>RXNT Info</v>
       </c>
-      <c r="K1" t="str">
+      <c r="M1" t="str">
         <v>WR</v>
       </c>
-      <c r="L1" t="str">
+      <c r="N1" t="str">
         <v>Hospice</v>
       </c>
-      <c r="M1" t="str">
+      <c r="O1" t="str">
         <v>Prescription Submit</v>
       </c>
-      <c r="N1" t="str">
-        <v/>
-      </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
+        <v/>
+      </c>
+      <c r="Q1" t="str">
         <v>invoice amount</v>
       </c>
-      <c r="P1" t="str">
+      <c r="R1" t="str">
         <v>PAID</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="S1" t="str">
         <v>Check list</v>
       </c>
-      <c r="R1" t="str">
+      <c r="T1" t="str">
         <v>Ingestion Date</v>
       </c>
-      <c r="S1" t="str">
+      <c r="U1" t="str">
         <v>Ingestion Location</v>
       </c>
-      <c r="T1" t="str">
+      <c r="V1" t="str">
         <v>TTS (Minutes)</v>
       </c>
-      <c r="U1" t="str">
+      <c r="W1" t="str">
         <v>TTD (Minutes)</v>
       </c>
-      <c r="V1" t="str">
+      <c r="X1" t="str">
         <v>Consent Received</v>
       </c>
-      <c r="W1" t="str">
+      <c r="Y1" t="str">
         <v>Medical Records</v>
       </c>
-      <c r="X1" t="str">
+      <c r="Z1" t="str">
         <v>Physician follow up form</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="AA1" t="str">
         <v>EOLOA State</v>
       </c>
-      <c r="Z1" t="str">
-        <v/>
-      </c>
-      <c r="AA1" t="str">
-        <v/>
-      </c>
       <c r="AB1" t="str">
         <v/>
       </c>
@@ -3192,6 +3258,12 @@
         <v/>
       </c>
       <c r="AD1" t="str">
+        <v/>
+      </c>
+      <c r="AE1" t="str">
+        <v/>
+      </c>
+      <c r="AF1" t="str">
         <v>Referred From</v>
       </c>
     </row>
@@ -3212,50 +3284,50 @@
         <v>45231</v>
       </c>
       <c r="F2" t="str">
+        <v>442-450-8177</v>
+      </c>
+      <c r="G2" t="str">
+        <v>phil.spektor@yahoo.com</v>
+      </c>
+      <c r="H2" t="str">
         <v>45261</v>
       </c>
-      <c r="G2" t="str">
+      <c r="I2" t="str">
         <v>Dr. karl Steinber</v>
       </c>
-      <c r="H2" t="str">
+      <c r="J2" t="str">
         <v>45505</v>
       </c>
-      <c r="I2" t="str">
+      <c r="K2" t="str">
         <v>45550</v>
       </c>
-      <c r="J2" t="str">
-        <v>yes</v>
-      </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
+        <v>yes</v>
+      </c>
+      <c r="M2" t="str">
         <v>44928</v>
       </c>
-      <c r="L2" t="str">
-        <v/>
-      </c>
-      <c r="M2" t="str">
+      <c r="N2" t="str">
+        <v/>
+      </c>
+      <c r="O2" t="str">
         <v>45271</v>
       </c>
-      <c r="N2" t="str">
-        <v/>
-      </c>
-      <c r="O2" t="str">
+      <c r="P2" t="str">
+        <v/>
+      </c>
+      <c r="Q2" t="str">
         <v>4125</v>
       </c>
-      <c r="P2" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Q2" t="str">
-        <v/>
-      </c>
       <c r="R2" t="str">
+        <v>yes</v>
+      </c>
+      <c r="S2" t="str">
+        <v/>
+      </c>
+      <c r="T2" t="str">
         <v>private home</v>
       </c>
-      <c r="S2" t="str">
-        <v/>
-      </c>
-      <c r="T2" t="str">
-        <v/>
-      </c>
       <c r="U2" t="str">
         <v/>
       </c>
@@ -3284,6 +3356,12 @@
         <v/>
       </c>
       <c r="AD2" t="str">
+        <v/>
+      </c>
+      <c r="AE2" t="str">
+        <v/>
+      </c>
+      <c r="AF2" t="str">
         <v/>
       </c>
     </row>
@@ -3307,22 +3385,22 @@
         <v/>
       </c>
       <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <v/>
+      </c>
+      <c r="I3" t="str">
         <v>Dr. Susan Bodtkiski</v>
       </c>
-      <c r="H3" t="str">
+      <c r="J3" t="str">
         <v>45518</v>
       </c>
-      <c r="I3" t="str">
+      <c r="K3" t="str">
         <v>45263</v>
       </c>
-      <c r="J3" t="str">
-        <v>yes</v>
-      </c>
-      <c r="K3" t="str">
-        <v/>
-      </c>
       <c r="L3" t="str">
-        <v/>
+        <v>yes</v>
       </c>
       <c r="M3" t="str">
         <v/>
@@ -3355,17 +3433,17 @@
         <v/>
       </c>
       <c r="W3" t="str">
-        <v>yes</v>
+        <v/>
       </c>
       <c r="X3" t="str">
+        <v/>
+      </c>
+      <c r="Y3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="Z3" t="str">
         <v>45160</v>
       </c>
-      <c r="Y3" t="str">
-        <v/>
-      </c>
-      <c r="Z3" t="str">
-        <v/>
-      </c>
       <c r="AA3" t="str">
         <v/>
       </c>
@@ -3376,6 +3454,12 @@
         <v/>
       </c>
       <c r="AD3" t="str">
+        <v/>
+      </c>
+      <c r="AE3" t="str">
+        <v/>
+      </c>
+      <c r="AF3" t="str">
         <v/>
       </c>
     </row>
@@ -3396,53 +3480,53 @@
         <v>San Diego</v>
       </c>
       <c r="F4" t="str">
+        <v>213-321-8235</v>
+      </c>
+      <c r="G4" t="str">
+        <v>rquinn@aol.com</v>
+      </c>
+      <c r="H4" t="str">
         <v>45722</v>
       </c>
-      <c r="G4" t="str">
+      <c r="I4" t="str">
         <v>45724</v>
       </c>
-      <c r="H4" t="str">
+      <c r="J4" t="str">
         <v>Dr. Lisa Green</v>
       </c>
-      <c r="I4" t="str">
+      <c r="K4" t="str">
         <v>45726</v>
       </c>
-      <c r="J4" t="str">
+      <c r="L4" t="str">
         <v>pending</v>
       </c>
-      <c r="K4" t="str">
+      <c r="M4" t="str">
         <v>45723</v>
       </c>
-      <c r="L4" t="str">
-        <v>yes</v>
-      </c>
-      <c r="M4" t="str">
+      <c r="N4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="O4" t="str">
         <v>Radiant</v>
       </c>
-      <c r="N4" t="str">
+      <c r="P4" t="str">
         <v>45727</v>
       </c>
-      <c r="O4" t="str">
-        <v/>
-      </c>
-      <c r="P4" t="str">
+      <c r="Q4" t="str">
+        <v/>
+      </c>
+      <c r="R4" t="str">
         <v>3700</v>
       </c>
-      <c r="Q4" t="str">
+      <c r="S4" t="str">
         <v>no</v>
       </c>
-      <c r="R4" t="str">
+      <c r="T4" t="str">
         <v>in progress</v>
       </c>
-      <c r="S4" t="str">
+      <c r="U4" t="str">
         <v>private home</v>
       </c>
-      <c r="T4" t="str">
-        <v/>
-      </c>
-      <c r="U4" t="str">
-        <v/>
-      </c>
       <c r="V4" t="str">
         <v/>
       </c>
@@ -3471,6 +3555,12 @@
         <v/>
       </c>
       <c r="AE4" t="str">
+        <v/>
+      </c>
+      <c r="AF4" t="str">
+        <v/>
+      </c>
+      <c r="AG4" t="str">
         <v>Radiant Hospice</v>
       </c>
     </row>
@@ -3491,53 +3581,53 @@
         <v>La Jolla</v>
       </c>
       <c r="F5" t="str">
+        <v>323-183-7928</v>
+      </c>
+      <c r="G5" t="str">
+        <v>steve921@outlook.com</v>
+      </c>
+      <c r="H5" t="str">
         <v>45727</v>
       </c>
-      <c r="G5" t="str">
+      <c r="I5" t="str">
         <v>45729</v>
       </c>
-      <c r="H5" t="str">
+      <c r="J5" t="str">
         <v>Dr. Mark Hale</v>
       </c>
-      <c r="I5" t="str">
+      <c r="K5" t="str">
         <v>45731</v>
       </c>
-      <c r="J5" t="str">
+      <c r="L5" t="str">
         <v>pending</v>
       </c>
-      <c r="K5" t="str">
+      <c r="M5" t="str">
         <v>45728</v>
       </c>
-      <c r="L5" t="str">
+      <c r="N5" t="str">
         <v>no</v>
       </c>
-      <c r="M5" t="str">
+      <c r="O5" t="str">
         <v>Serenity Hospice</v>
       </c>
-      <c r="N5" t="str">
+      <c r="P5" t="str">
         <v>45732</v>
       </c>
-      <c r="O5" t="str">
-        <v/>
-      </c>
-      <c r="P5" t="str">
+      <c r="Q5" t="str">
+        <v/>
+      </c>
+      <c r="R5" t="str">
         <v>3000</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="S5" t="str">
         <v>no</v>
       </c>
-      <c r="R5" t="str">
+      <c r="T5" t="str">
         <v>in progress</v>
       </c>
-      <c r="S5" t="str">
+      <c r="U5" t="str">
         <v>assisted living</v>
       </c>
-      <c r="T5" t="str">
-        <v/>
-      </c>
-      <c r="U5" t="str">
-        <v/>
-      </c>
       <c r="V5" t="str">
         <v/>
       </c>
@@ -3566,6 +3656,12 @@
         <v/>
       </c>
       <c r="AE5" t="str">
+        <v/>
+      </c>
+      <c r="AF5" t="str">
+        <v/>
+      </c>
+      <c r="AG5" t="str">
         <v>Serenity Hospice</v>
       </c>
     </row>
@@ -3586,53 +3682,53 @@
         <v>Encinitas</v>
       </c>
       <c r="F6" t="str">
+        <v>442-709-5063</v>
+      </c>
+      <c r="G6" t="str">
+        <v>tina.santos@hotmail.com</v>
+      </c>
+      <c r="H6" t="str">
         <v>45732</v>
       </c>
-      <c r="G6" t="str">
+      <c r="I6" t="str">
         <v>45734</v>
       </c>
-      <c r="H6" t="str">
+      <c r="J6" t="str">
         <v>Dr. Nina Ford</v>
       </c>
-      <c r="I6" t="str">
+      <c r="K6" t="str">
         <v>45736</v>
       </c>
-      <c r="J6" t="str">
+      <c r="L6" t="str">
         <v>pending</v>
       </c>
-      <c r="K6" t="str">
+      <c r="M6" t="str">
         <v>45733</v>
       </c>
-      <c r="L6" t="str">
-        <v>yes</v>
-      </c>
-      <c r="M6" t="str">
+      <c r="N6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="O6" t="str">
         <v>Harmony Care</v>
       </c>
-      <c r="N6" t="str">
+      <c r="P6" t="str">
         <v>45737</v>
       </c>
-      <c r="O6" t="str">
-        <v/>
-      </c>
-      <c r="P6" t="str">
+      <c r="Q6" t="str">
+        <v/>
+      </c>
+      <c r="R6" t="str">
         <v>4000</v>
       </c>
-      <c r="Q6" t="str">
+      <c r="S6" t="str">
         <v>no</v>
       </c>
-      <c r="R6" t="str">
+      <c r="T6" t="str">
         <v>in progress</v>
       </c>
-      <c r="S6" t="str">
+      <c r="U6" t="str">
         <v>acute care hospital</v>
       </c>
-      <c r="T6" t="str">
-        <v/>
-      </c>
-      <c r="U6" t="str">
-        <v/>
-      </c>
       <c r="V6" t="str">
         <v/>
       </c>
@@ -3661,6 +3757,12 @@
         <v/>
       </c>
       <c r="AE6" t="str">
+        <v/>
+      </c>
+      <c r="AF6" t="str">
+        <v/>
+      </c>
+      <c r="AG6" t="str">
         <v>Harmony Care</v>
       </c>
     </row>
@@ -3681,53 +3783,53 @@
         <v>Oceanside</v>
       </c>
       <c r="F7" t="str">
+        <v>760-335-2451</v>
+      </c>
+      <c r="G7" t="str">
+        <v>utorres@gmail.com</v>
+      </c>
+      <c r="H7" t="str">
         <v>45737</v>
       </c>
-      <c r="G7" t="str">
+      <c r="I7" t="str">
         <v>45739</v>
       </c>
-      <c r="H7" t="str">
+      <c r="J7" t="str">
         <v>Dr. Owen Gray</v>
       </c>
-      <c r="I7" t="str">
+      <c r="K7" t="str">
         <v>45741</v>
       </c>
-      <c r="J7" t="str">
+      <c r="L7" t="str">
         <v>pending</v>
       </c>
-      <c r="K7" t="str">
+      <c r="M7" t="str">
         <v>45738</v>
       </c>
-      <c r="L7" t="str">
+      <c r="N7" t="str">
         <v>no</v>
       </c>
-      <c r="M7" t="str">
+      <c r="O7" t="str">
         <v>Coastal Hospice</v>
       </c>
-      <c r="N7" t="str">
+      <c r="P7" t="str">
         <v>45742</v>
       </c>
-      <c r="O7" t="str">
-        <v/>
-      </c>
-      <c r="P7" t="str">
+      <c r="Q7" t="str">
+        <v/>
+      </c>
+      <c r="R7" t="str">
         <v>3200</v>
       </c>
-      <c r="Q7" t="str">
+      <c r="S7" t="str">
         <v>no</v>
       </c>
-      <c r="R7" t="str">
+      <c r="T7" t="str">
         <v>in progress</v>
       </c>
-      <c r="S7" t="str">
+      <c r="U7" t="str">
         <v>in-patient hospice</v>
       </c>
-      <c r="T7" t="str">
-        <v/>
-      </c>
-      <c r="U7" t="str">
-        <v/>
-      </c>
       <c r="V7" t="str">
         <v/>
       </c>
@@ -3756,6 +3858,12 @@
         <v/>
       </c>
       <c r="AE7" t="str">
+        <v/>
+      </c>
+      <c r="AF7" t="str">
+        <v/>
+      </c>
+      <c r="AG7" t="str">
         <v>Coastal Hospice</v>
       </c>
     </row>
@@ -3776,53 +3884,53 @@
         <v>Carlsbad</v>
       </c>
       <c r="F8" t="str">
+        <v>619-317-1799</v>
+      </c>
+      <c r="G8" t="str">
+        <v>victoria_underwood@aol.com</v>
+      </c>
+      <c r="H8" t="str">
         <v>45742</v>
       </c>
-      <c r="G8" t="str">
+      <c r="I8" t="str">
         <v>45744</v>
       </c>
-      <c r="H8" t="str">
+      <c r="J8" t="str">
         <v>Dr. Paula Hunt</v>
       </c>
-      <c r="I8" t="str">
+      <c r="K8" t="str">
         <v>45746</v>
       </c>
-      <c r="J8" t="str">
+      <c r="L8" t="str">
         <v>pending</v>
       </c>
-      <c r="K8" t="str">
+      <c r="M8" t="str">
         <v>45743</v>
       </c>
-      <c r="L8" t="str">
-        <v>yes</v>
-      </c>
-      <c r="M8" t="str">
+      <c r="N8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="O8" t="str">
         <v>Sunrise Hospice</v>
       </c>
-      <c r="N8" t="str">
+      <c r="P8" t="str">
         <v>45747</v>
       </c>
-      <c r="O8" t="str">
-        <v/>
-      </c>
-      <c r="P8" t="str">
+      <c r="Q8" t="str">
+        <v/>
+      </c>
+      <c r="R8" t="str">
         <v>3900</v>
       </c>
-      <c r="Q8" t="str">
+      <c r="S8" t="str">
         <v>no</v>
       </c>
-      <c r="R8" t="str">
+      <c r="T8" t="str">
         <v>in progress</v>
       </c>
-      <c r="S8" t="str">
+      <c r="U8" t="str">
         <v>other</v>
       </c>
-      <c r="T8" t="str">
-        <v/>
-      </c>
-      <c r="U8" t="str">
-        <v/>
-      </c>
       <c r="V8" t="str">
         <v/>
       </c>
@@ -3851,6 +3959,12 @@
         <v/>
       </c>
       <c r="AE8" t="str">
+        <v/>
+      </c>
+      <c r="AF8" t="str">
+        <v/>
+      </c>
+      <c r="AG8" t="str">
         <v>Sunrise Hospice</v>
       </c>
     </row>
@@ -3871,53 +3985,53 @@
         <v>Del Mar</v>
       </c>
       <c r="F9" t="str">
+        <v>562-211-7829</v>
+      </c>
+      <c r="G9" t="str">
+        <v>williamvargas@outlook.com</v>
+      </c>
+      <c r="H9" t="str">
         <v>45747</v>
       </c>
-      <c r="G9" t="str">
+      <c r="I9" t="str">
         <v>45749</v>
       </c>
-      <c r="H9" t="str">
+      <c r="J9" t="str">
         <v>Dr. Quentin Ives</v>
       </c>
-      <c r="I9" t="str">
+      <c r="K9" t="str">
         <v>45751</v>
       </c>
-      <c r="J9" t="str">
+      <c r="L9" t="str">
         <v>pending</v>
       </c>
-      <c r="K9" t="str">
+      <c r="M9" t="str">
         <v>45748</v>
       </c>
-      <c r="L9" t="str">
+      <c r="N9" t="str">
         <v>no</v>
       </c>
-      <c r="M9" t="str">
+      <c r="O9" t="str">
         <v>Eternal Peace</v>
       </c>
-      <c r="N9" t="str">
+      <c r="P9" t="str">
         <v>45752</v>
       </c>
-      <c r="O9" t="str">
-        <v/>
-      </c>
-      <c r="P9" t="str">
+      <c r="Q9" t="str">
+        <v/>
+      </c>
+      <c r="R9" t="str">
         <v>4300</v>
       </c>
-      <c r="Q9" t="str">
+      <c r="S9" t="str">
         <v>no</v>
       </c>
-      <c r="R9" t="str">
+      <c r="T9" t="str">
         <v>in progress</v>
       </c>
-      <c r="S9" t="str">
+      <c r="U9" t="str">
         <v>private home</v>
       </c>
-      <c r="T9" t="str">
-        <v/>
-      </c>
-      <c r="U9" t="str">
-        <v/>
-      </c>
       <c r="V9" t="str">
         <v/>
       </c>
@@ -3946,6 +4060,12 @@
         <v/>
       </c>
       <c r="AE9" t="str">
+        <v/>
+      </c>
+      <c r="AF9" t="str">
+        <v/>
+      </c>
+      <c r="AG9" t="str">
         <v>Eternal Peace</v>
       </c>
     </row>
@@ -3966,53 +4086,53 @@
         <v>Vista</v>
       </c>
       <c r="F10" t="str">
+        <v>619-367-4098</v>
+      </c>
+      <c r="G10" t="str">
+        <v>xena.valdez@hotmail.com</v>
+      </c>
+      <c r="H10" t="str">
         <v>45752</v>
       </c>
-      <c r="G10" t="str">
+      <c r="I10" t="str">
         <v>45754</v>
       </c>
-      <c r="H10" t="str">
+      <c r="J10" t="str">
         <v>Dr. Rachel James</v>
       </c>
-      <c r="I10" t="str">
+      <c r="K10" t="str">
         <v>45756</v>
       </c>
-      <c r="J10" t="str">
+      <c r="L10" t="str">
         <v>pending</v>
       </c>
-      <c r="K10" t="str">
+      <c r="M10" t="str">
         <v>45753</v>
       </c>
-      <c r="L10" t="str">
-        <v>yes</v>
-      </c>
-      <c r="M10" t="str">
+      <c r="N10" t="str">
+        <v>yes</v>
+      </c>
+      <c r="O10" t="str">
         <v>Tranquil Care</v>
       </c>
-      <c r="N10" t="str">
+      <c r="P10" t="str">
         <v>45757</v>
       </c>
-      <c r="O10" t="str">
-        <v/>
-      </c>
-      <c r="P10" t="str">
+      <c r="Q10" t="str">
+        <v/>
+      </c>
+      <c r="R10" t="str">
         <v>3400</v>
       </c>
-      <c r="Q10" t="str">
+      <c r="S10" t="str">
         <v>no</v>
       </c>
-      <c r="R10" t="str">
+      <c r="T10" t="str">
         <v>in progress</v>
       </c>
-      <c r="S10" t="str">
+      <c r="U10" t="str">
         <v>assisted living</v>
       </c>
-      <c r="T10" t="str">
-        <v/>
-      </c>
-      <c r="U10" t="str">
-        <v/>
-      </c>
       <c r="V10" t="str">
         <v/>
       </c>
@@ -4041,6 +4161,12 @@
         <v/>
       </c>
       <c r="AE10" t="str">
+        <v/>
+      </c>
+      <c r="AF10" t="str">
+        <v/>
+      </c>
+      <c r="AG10" t="str">
         <v>Tranquil Care</v>
       </c>
     </row>
@@ -4061,53 +4187,53 @@
         <v>Escondido</v>
       </c>
       <c r="F11" t="str">
+        <v>760-710-6342</v>
+      </c>
+      <c r="G11" t="str">
+        <v>yosef.vasquez@hotmail.com</v>
+      </c>
+      <c r="H11" t="str">
         <v>45757</v>
       </c>
-      <c r="G11" t="str">
+      <c r="I11" t="str">
         <v>45759</v>
       </c>
-      <c r="H11" t="str">
+      <c r="J11" t="str">
         <v>Dr. Sam Kline</v>
       </c>
-      <c r="I11" t="str">
+      <c r="K11" t="str">
         <v>45761</v>
       </c>
-      <c r="J11" t="str">
+      <c r="L11" t="str">
         <v>pending</v>
       </c>
-      <c r="K11" t="str">
+      <c r="M11" t="str">
         <v>45758</v>
       </c>
-      <c r="L11" t="str">
+      <c r="N11" t="str">
         <v>no</v>
       </c>
-      <c r="M11" t="str">
+      <c r="O11" t="str">
         <v>Peaceful End</v>
       </c>
-      <c r="N11" t="str">
+      <c r="P11" t="str">
         <v>45762</v>
       </c>
-      <c r="O11" t="str">
-        <v/>
-      </c>
-      <c r="P11" t="str">
+      <c r="Q11" t="str">
+        <v/>
+      </c>
+      <c r="R11" t="str">
         <v>4100</v>
       </c>
-      <c r="Q11" t="str">
+      <c r="S11" t="str">
         <v>no</v>
       </c>
-      <c r="R11" t="str">
+      <c r="T11" t="str">
         <v>in progress</v>
       </c>
-      <c r="S11" t="str">
+      <c r="U11" t="str">
         <v>acute care hospital</v>
       </c>
-      <c r="T11" t="str">
-        <v/>
-      </c>
-      <c r="U11" t="str">
-        <v/>
-      </c>
       <c r="V11" t="str">
         <v/>
       </c>
@@ -4136,12 +4262,18 @@
         <v/>
       </c>
       <c r="AE11" t="str">
+        <v/>
+      </c>
+      <c r="AF11" t="str">
+        <v/>
+      </c>
+      <c r="AG11" t="str">
         <v>Peaceful End</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AG11"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -4782,7 +4914,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -5109,9 +5241,29 @@
         <v>introduction</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>20250803030334</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Alyssa</v>
+      </c>
+      <c r="C15" t="str">
+        <v>test</v>
+      </c>
+      <c r="D15" t="str">
+        <v>GM</v>
+      </c>
+      <c r="E15" t="str">
+        <v>all</v>
+      </c>
+      <c r="F15" t="str">
+        <v>active</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feature/chat recipients checkbox (#1)
* Add Vendors tab with 6 sample service partner companies for hospice management

* Add Vendors section to UI with beautiful card layout and category grouping

* Add task tabs for Christa and Amber to user section

* Add Team Chat functionality with XLSX storage and @mentions support

* Implement advanced chat system with DM/Group messages, user coding, and participant filtering

* Fix chat loading error and implement Alyssa's perspective view with user switching

* chore(test): add agent smoke test

* docs(rules): tighten non-interactive defaults; cleanup test artifacts

* feat(chat): recipients checkbox selector, user color-coding, and XLSX-aligned message write; non-breaking UI CSS

* chore(test): auth push check
</commit_message>
<xml_diff>
--- a/Dashboard Clone.xlsx
+++ b/Dashboard Clone.xlsx
@@ -9,6 +9,8 @@
     <sheet name="Closed" sheetId="4" r:id="rId4"/>
     <sheet name="Oustanding" sheetId="5" r:id="rId5"/>
     <sheet name="Call Log" sheetId="6" r:id="rId6"/>
+    <sheet name="Vendors" sheetId="7" r:id="rId7"/>
+    <sheet name="Chat" sheetId="8" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -402,9 +404,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:AH11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -427,78 +429,84 @@
         <v>Area</v>
       </c>
       <c r="G1" t="str">
+        <v>Phone Number</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="I1" t="str">
         <v>1st request</v>
       </c>
-      <c r="H1" t="str">
+      <c r="J1" t="str">
         <v>2nd request</v>
       </c>
-      <c r="I1" t="str">
+      <c r="K1" t="str">
         <v>CP Doctor</v>
       </c>
-      <c r="J1" t="str">
+      <c r="L1" t="str">
         <v>CP Completed</v>
       </c>
-      <c r="K1" t="str">
+      <c r="M1" t="str">
         <v>RXNT Info</v>
       </c>
-      <c r="L1" t="str">
+      <c r="N1" t="str">
         <v>WR</v>
       </c>
-      <c r="M1" t="str">
+      <c r="O1" t="str">
         <v>Hospice</v>
       </c>
-      <c r="N1" t="str">
+      <c r="P1" t="str">
         <v>Prescription Submit</v>
       </c>
-      <c r="O1" t="str">
-        <v/>
-      </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
+        <v/>
+      </c>
+      <c r="R1" t="str">
         <v>invoice amount</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="S1" t="str">
         <v>PAID</v>
       </c>
-      <c r="R1" t="str">
+      <c r="T1" t="str">
         <v>Check list</v>
       </c>
-      <c r="S1" t="str">
+      <c r="U1" t="str">
         <v>Ingestion Date</v>
       </c>
-      <c r="T1" t="str">
+      <c r="V1" t="str">
         <v>Ingestion Location</v>
       </c>
-      <c r="U1" t="str">
+      <c r="W1" t="str">
         <v>TTS (Minutes)</v>
       </c>
-      <c r="V1" t="str">
+      <c r="X1" t="str">
         <v>TTD (Minutes)</v>
       </c>
-      <c r="W1" t="str">
+      <c r="Y1" t="str">
         <v>Consent Received</v>
       </c>
-      <c r="X1" t="str">
+      <c r="Z1" t="str">
         <v>Medical Records</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="AA1" t="str">
         <v>Physician follow up form</v>
       </c>
-      <c r="Z1" t="str">
+      <c r="AB1" t="str">
         <v>EOLOA State</v>
       </c>
-      <c r="AA1" t="str">
+      <c r="AC1" t="str">
         <v>Death Certificate</v>
       </c>
-      <c r="AB1" t="str">
+      <c r="AD1" t="str">
         <v>All Recodrs in DRC</v>
       </c>
-      <c r="AC1" t="str">
-        <v/>
-      </c>
-      <c r="AD1" t="str">
+      <c r="AE1" t="str">
+        <v/>
+      </c>
+      <c r="AF1" t="str">
         <v>Riverside EOLOA</v>
       </c>
-      <c r="AE1" t="str">
+      <c r="AG1" t="str">
         <v>Referred From</v>
       </c>
     </row>
@@ -522,71 +530,71 @@
         <v>san diego</v>
       </c>
       <c r="G2" t="str">
+        <v>760-734-1214</v>
+      </c>
+      <c r="H2" t="str">
+        <v>adam255@hotmail.com</v>
+      </c>
+      <c r="I2" t="str">
         <v>45525</v>
       </c>
-      <c r="H2" t="str">
+      <c r="J2" t="str">
         <v>45527</v>
       </c>
-      <c r="I2" t="str">
+      <c r="K2" t="str">
         <v>Andzel</v>
       </c>
-      <c r="J2" t="str">
+      <c r="L2" t="str">
         <v>Gaja</v>
       </c>
-      <c r="K2" t="str">
+      <c r="M2" t="str">
         <v>45529</v>
       </c>
-      <c r="L2" t="str">
+      <c r="N2" t="str">
         <v>complete</v>
       </c>
-      <c r="M2" t="str">
+      <c r="O2" t="str">
         <v>45525</v>
       </c>
-      <c r="N2" t="str">
+      <c r="P2" t="str">
         <v>Radiant</v>
       </c>
-      <c r="O2" t="str">
+      <c r="Q2" t="str">
         <v>45530</v>
       </c>
-      <c r="P2" t="str">
-        <v/>
-      </c>
-      <c r="Q2" t="str">
+      <c r="R2" t="str">
+        <v/>
+      </c>
+      <c r="S2" t="str">
         <v>4200</v>
       </c>
-      <c r="R2" t="str">
-        <v>yes</v>
-      </c>
-      <c r="S2" t="str">
+      <c r="T2" t="str">
+        <v>yes</v>
+      </c>
+      <c r="U2" t="str">
         <v>complete</v>
       </c>
-      <c r="T2" t="str">
+      <c r="V2" t="str">
         <v>45536</v>
       </c>
-      <c r="U2" t="str">
+      <c r="W2" t="str">
         <v>residents</v>
       </c>
-      <c r="V2" t="str">
+      <c r="X2" t="str">
         <v>3</v>
       </c>
-      <c r="W2" t="str">
+      <c r="Y2" t="str">
         <v>64</v>
       </c>
-      <c r="X2" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y2" t="str">
-        <v>yes</v>
-      </c>
       <c r="Z2" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA2" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB2" t="str">
         <v>45545</v>
       </c>
-      <c r="AA2" t="str">
-        <v/>
-      </c>
-      <c r="AB2" t="str">
-        <v/>
-      </c>
       <c r="AC2" t="str">
         <v/>
       </c>
@@ -597,6 +605,12 @@
         <v/>
       </c>
       <c r="AF2" t="str">
+        <v/>
+      </c>
+      <c r="AG2" t="str">
+        <v/>
+      </c>
+      <c r="AH2" t="str">
         <v>Radiant Hospice</v>
       </c>
     </row>
@@ -620,14 +634,14 @@
         <v>La Jolla</v>
       </c>
       <c r="G3" t="str">
+        <v>951-218-4377</v>
+      </c>
+      <c r="H3" t="str">
+        <v>clare_burd@aol.com</v>
+      </c>
+      <c r="I3" t="str">
         <v>45720</v>
       </c>
-      <c r="H3" t="str">
-        <v/>
-      </c>
-      <c r="I3" t="str">
-        <v/>
-      </c>
       <c r="J3" t="str">
         <v/>
       </c>
@@ -692,6 +706,12 @@
         <v/>
       </c>
       <c r="AE3" t="str">
+        <v/>
+      </c>
+      <c r="AF3" t="str">
+        <v/>
+      </c>
+      <c r="AG3" t="str">
         <v/>
       </c>
     </row>
@@ -715,71 +735,71 @@
         <v>Encinitas</v>
       </c>
       <c r="G4" t="str">
+        <v>714-357-6734</v>
+      </c>
+      <c r="H4" t="str">
+        <v>emily_carter@yahoo.com</v>
+      </c>
+      <c r="I4" t="str">
         <v>45722</v>
       </c>
-      <c r="H4" t="str">
+      <c r="J4" t="str">
         <v>45724</v>
       </c>
-      <c r="I4" t="str">
+      <c r="K4" t="str">
         <v>Dr. Lisa Green</v>
       </c>
-      <c r="J4" t="str">
+      <c r="L4" t="str">
         <v>45726</v>
       </c>
-      <c r="K4" t="str">
+      <c r="M4" t="str">
         <v>complete</v>
       </c>
-      <c r="L4" t="str">
+      <c r="N4" t="str">
         <v>45723</v>
       </c>
-      <c r="M4" t="str">
-        <v>yes</v>
-      </c>
-      <c r="N4" t="str">
+      <c r="O4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="P4" t="str">
         <v>Serenity Hospice</v>
       </c>
-      <c r="O4" t="str">
+      <c r="Q4" t="str">
         <v>45727</v>
       </c>
-      <c r="P4" t="str">
-        <v/>
-      </c>
-      <c r="Q4" t="str">
+      <c r="R4" t="str">
+        <v/>
+      </c>
+      <c r="S4" t="str">
         <v>3500</v>
       </c>
-      <c r="R4" t="str">
-        <v>yes</v>
-      </c>
-      <c r="S4" t="str">
+      <c r="T4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="U4" t="str">
         <v>complete</v>
       </c>
-      <c r="T4" t="str">
+      <c r="V4" t="str">
         <v>45730</v>
       </c>
-      <c r="U4" t="str">
+      <c r="W4" t="str">
         <v>private home</v>
       </c>
-      <c r="V4" t="str">
+      <c r="X4" t="str">
         <v>5</v>
       </c>
-      <c r="W4" t="str">
+      <c r="Y4" t="str">
         <v>45</v>
       </c>
-      <c r="X4" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y4" t="str">
-        <v>yes</v>
-      </c>
       <c r="Z4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB4" t="str">
         <v>45735</v>
       </c>
-      <c r="AA4" t="str">
-        <v/>
-      </c>
-      <c r="AB4" t="str">
-        <v/>
-      </c>
       <c r="AC4" t="str">
         <v/>
       </c>
@@ -790,6 +810,12 @@
         <v/>
       </c>
       <c r="AF4" t="str">
+        <v/>
+      </c>
+      <c r="AG4" t="str">
+        <v/>
+      </c>
+      <c r="AH4" t="str">
         <v>Serenity Hospice</v>
       </c>
     </row>
@@ -813,71 +839,71 @@
         <v>San Diego</v>
       </c>
       <c r="G5" t="str">
+        <v>714-700-7058</v>
+      </c>
+      <c r="H5" t="str">
+        <v>frank.davis@hotmail.com</v>
+      </c>
+      <c r="I5" t="str">
         <v>45727</v>
       </c>
-      <c r="H5" t="str">
+      <c r="J5" t="str">
         <v>45729</v>
       </c>
-      <c r="I5" t="str">
+      <c r="K5" t="str">
         <v>Dr. Mark Hale</v>
       </c>
-      <c r="J5" t="str">
+      <c r="L5" t="str">
         <v>45731</v>
       </c>
-      <c r="K5" t="str">
+      <c r="M5" t="str">
         <v>pending</v>
       </c>
-      <c r="L5" t="str">
+      <c r="N5" t="str">
         <v>45728</v>
       </c>
-      <c r="M5" t="str">
+      <c r="O5" t="str">
         <v>no</v>
       </c>
-      <c r="N5" t="str">
+      <c r="P5" t="str">
         <v>Radiant</v>
       </c>
-      <c r="O5" t="str">
+      <c r="Q5" t="str">
         <v>45732</v>
       </c>
-      <c r="P5" t="str">
-        <v/>
-      </c>
-      <c r="Q5" t="str">
+      <c r="R5" t="str">
+        <v/>
+      </c>
+      <c r="S5" t="str">
         <v>2800</v>
       </c>
-      <c r="R5" t="str">
+      <c r="T5" t="str">
         <v>no</v>
       </c>
-      <c r="S5" t="str">
+      <c r="U5" t="str">
         <v>in progress</v>
       </c>
-      <c r="T5" t="str">
+      <c r="V5" t="str">
         <v>45735</v>
       </c>
-      <c r="U5" t="str">
+      <c r="W5" t="str">
         <v>assisted living</v>
       </c>
-      <c r="V5" t="str">
+      <c r="X5" t="str">
         <v>10</v>
       </c>
-      <c r="W5" t="str">
+      <c r="Y5" t="str">
         <v>120</v>
       </c>
-      <c r="X5" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y5" t="str">
+      <c r="Z5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA5" t="str">
         <v>no</v>
       </c>
-      <c r="Z5" t="str">
+      <c r="AB5" t="str">
         <v>45740</v>
       </c>
-      <c r="AA5" t="str">
-        <v/>
-      </c>
-      <c r="AB5" t="str">
-        <v/>
-      </c>
       <c r="AC5" t="str">
         <v/>
       </c>
@@ -888,6 +914,12 @@
         <v/>
       </c>
       <c r="AF5" t="str">
+        <v/>
+      </c>
+      <c r="AG5" t="str">
+        <v/>
+      </c>
+      <c r="AH5" t="str">
         <v>Radiant Hospice</v>
       </c>
     </row>
@@ -911,71 +943,71 @@
         <v>La Jolla</v>
       </c>
       <c r="G6" t="str">
+        <v>714-500-4286</v>
+      </c>
+      <c r="H6" t="str">
+        <v>grace_evans@hotmail.com</v>
+      </c>
+      <c r="I6" t="str">
         <v>45732</v>
       </c>
-      <c r="H6" t="str">
+      <c r="J6" t="str">
         <v>45734</v>
       </c>
-      <c r="I6" t="str">
+      <c r="K6" t="str">
         <v>Dr. Nina Ford</v>
       </c>
-      <c r="J6" t="str">
+      <c r="L6" t="str">
         <v>45736</v>
       </c>
-      <c r="K6" t="str">
+      <c r="M6" t="str">
         <v>complete</v>
       </c>
-      <c r="L6" t="str">
+      <c r="N6" t="str">
         <v>45733</v>
       </c>
-      <c r="M6" t="str">
-        <v>yes</v>
-      </c>
-      <c r="N6" t="str">
+      <c r="O6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="P6" t="str">
         <v>Harmony Care</v>
       </c>
-      <c r="O6" t="str">
+      <c r="Q6" t="str">
         <v>45737</v>
       </c>
-      <c r="P6" t="str">
-        <v/>
-      </c>
-      <c r="Q6" t="str">
+      <c r="R6" t="str">
+        <v/>
+      </c>
+      <c r="S6" t="str">
         <v>4100</v>
       </c>
-      <c r="R6" t="str">
-        <v>yes</v>
-      </c>
-      <c r="S6" t="str">
+      <c r="T6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="U6" t="str">
         <v>complete</v>
       </c>
-      <c r="T6" t="str">
+      <c r="V6" t="str">
         <v>45740</v>
       </c>
-      <c r="U6" t="str">
+      <c r="W6" t="str">
         <v>residents</v>
       </c>
-      <c r="V6" t="str">
+      <c r="X6" t="str">
         <v>2</v>
       </c>
-      <c r="W6" t="str">
+      <c r="Y6" t="str">
         <v>30</v>
       </c>
-      <c r="X6" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y6" t="str">
-        <v>yes</v>
-      </c>
       <c r="Z6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB6" t="str">
         <v>45745</v>
       </c>
-      <c r="AA6" t="str">
-        <v/>
-      </c>
-      <c r="AB6" t="str">
-        <v/>
-      </c>
       <c r="AC6" t="str">
         <v/>
       </c>
@@ -986,6 +1018,12 @@
         <v/>
       </c>
       <c r="AF6" t="str">
+        <v/>
+      </c>
+      <c r="AG6" t="str">
+        <v/>
+      </c>
+      <c r="AH6" t="str">
         <v>Harmony Care</v>
       </c>
     </row>
@@ -1009,71 +1047,71 @@
         <v>Oceanside</v>
       </c>
       <c r="G7" t="str">
+        <v>323-720-5970</v>
+      </c>
+      <c r="H7" t="str">
+        <v>henry_foster@yahoo.com</v>
+      </c>
+      <c r="I7" t="str">
         <v>45737</v>
       </c>
-      <c r="H7" t="str">
+      <c r="J7" t="str">
         <v>45739</v>
       </c>
-      <c r="I7" t="str">
+      <c r="K7" t="str">
         <v>Dr. Owen Gray</v>
       </c>
-      <c r="J7" t="str">
+      <c r="L7" t="str">
         <v>45741</v>
       </c>
-      <c r="K7" t="str">
+      <c r="M7" t="str">
         <v>complete</v>
       </c>
-      <c r="L7" t="str">
+      <c r="N7" t="str">
         <v>45738</v>
       </c>
-      <c r="M7" t="str">
+      <c r="O7" t="str">
         <v>no</v>
       </c>
-      <c r="N7" t="str">
+      <c r="P7" t="str">
         <v>Coastal Hospice</v>
       </c>
-      <c r="O7" t="str">
+      <c r="Q7" t="str">
         <v>45742</v>
       </c>
-      <c r="P7" t="str">
-        <v/>
-      </c>
-      <c r="Q7" t="str">
+      <c r="R7" t="str">
+        <v/>
+      </c>
+      <c r="S7" t="str">
         <v>3200</v>
       </c>
-      <c r="R7" t="str">
-        <v>yes</v>
-      </c>
-      <c r="S7" t="str">
+      <c r="T7" t="str">
+        <v>yes</v>
+      </c>
+      <c r="U7" t="str">
         <v>complete</v>
       </c>
-      <c r="T7" t="str">
+      <c r="V7" t="str">
         <v>45745</v>
       </c>
-      <c r="U7" t="str">
+      <c r="W7" t="str">
         <v>private home</v>
       </c>
-      <c r="V7" t="str">
+      <c r="X7" t="str">
         <v>4</v>
       </c>
-      <c r="W7" t="str">
+      <c r="Y7" t="str">
         <v>60</v>
       </c>
-      <c r="X7" t="str">
+      <c r="Z7" t="str">
         <v>no</v>
       </c>
-      <c r="Y7" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Z7" t="str">
+      <c r="AA7" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB7" t="str">
         <v>45750</v>
       </c>
-      <c r="AA7" t="str">
-        <v/>
-      </c>
-      <c r="AB7" t="str">
-        <v/>
-      </c>
       <c r="AC7" t="str">
         <v/>
       </c>
@@ -1084,6 +1122,12 @@
         <v/>
       </c>
       <c r="AF7" t="str">
+        <v/>
+      </c>
+      <c r="AG7" t="str">
+        <v/>
+      </c>
+      <c r="AH7" t="str">
         <v>Coastal Hospice</v>
       </c>
     </row>
@@ -1107,71 +1151,71 @@
         <v>Carlsbad</v>
       </c>
       <c r="G8" t="str">
+        <v>760-570-2681</v>
+      </c>
+      <c r="H8" t="str">
+        <v>igomez@outlook.com</v>
+      </c>
+      <c r="I8" t="str">
         <v>45742</v>
       </c>
-      <c r="H8" t="str">
+      <c r="J8" t="str">
         <v>45744</v>
       </c>
-      <c r="I8" t="str">
+      <c r="K8" t="str">
         <v>Dr. Paula Hunt</v>
       </c>
-      <c r="J8" t="str">
+      <c r="L8" t="str">
         <v>45746</v>
       </c>
-      <c r="K8" t="str">
+      <c r="M8" t="str">
         <v>pending</v>
       </c>
-      <c r="L8" t="str">
+      <c r="N8" t="str">
         <v>45743</v>
       </c>
-      <c r="M8" t="str">
-        <v>yes</v>
-      </c>
-      <c r="N8" t="str">
+      <c r="O8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="P8" t="str">
         <v>Sunrise Hospice</v>
       </c>
-      <c r="O8" t="str">
+      <c r="Q8" t="str">
         <v>45747</v>
       </c>
-      <c r="P8" t="str">
-        <v/>
-      </c>
-      <c r="Q8" t="str">
+      <c r="R8" t="str">
+        <v/>
+      </c>
+      <c r="S8" t="str">
         <v>3900</v>
       </c>
-      <c r="R8" t="str">
+      <c r="T8" t="str">
         <v>no</v>
       </c>
-      <c r="S8" t="str">
+      <c r="U8" t="str">
         <v>in progress</v>
       </c>
-      <c r="T8" t="str">
+      <c r="V8" t="str">
         <v>45750</v>
       </c>
-      <c r="U8" t="str">
+      <c r="W8" t="str">
         <v>acute care hospital</v>
       </c>
-      <c r="V8" t="str">
+      <c r="X8" t="str">
         <v>15</v>
       </c>
-      <c r="W8" t="str">
+      <c r="Y8" t="str">
         <v>180</v>
       </c>
-      <c r="X8" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y8" t="str">
-        <v>yes</v>
-      </c>
       <c r="Z8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB8" t="str">
         <v>45755</v>
       </c>
-      <c r="AA8" t="str">
-        <v/>
-      </c>
-      <c r="AB8" t="str">
-        <v/>
-      </c>
       <c r="AC8" t="str">
         <v/>
       </c>
@@ -1182,6 +1226,12 @@
         <v/>
       </c>
       <c r="AF8" t="str">
+        <v/>
+      </c>
+      <c r="AG8" t="str">
+        <v/>
+      </c>
+      <c r="AH8" t="str">
         <v>Sunrise Hospice</v>
       </c>
     </row>
@@ -1205,71 +1255,71 @@
         <v>Del Mar</v>
       </c>
       <c r="G9" t="str">
+        <v>323-618-5577</v>
+      </c>
+      <c r="H9" t="str">
+        <v>jackharris@yahoo.com</v>
+      </c>
+      <c r="I9" t="str">
         <v>45747</v>
       </c>
-      <c r="H9" t="str">
+      <c r="J9" t="str">
         <v>45749</v>
       </c>
-      <c r="I9" t="str">
+      <c r="K9" t="str">
         <v>Dr. Quentin Ives</v>
       </c>
-      <c r="J9" t="str">
+      <c r="L9" t="str">
         <v>45751</v>
       </c>
-      <c r="K9" t="str">
+      <c r="M9" t="str">
         <v>complete</v>
       </c>
-      <c r="L9" t="str">
+      <c r="N9" t="str">
         <v>45748</v>
       </c>
-      <c r="M9" t="str">
+      <c r="O9" t="str">
         <v>no</v>
       </c>
-      <c r="N9" t="str">
+      <c r="P9" t="str">
         <v>Eternal Peace</v>
       </c>
-      <c r="O9" t="str">
+      <c r="Q9" t="str">
         <v>45752</v>
       </c>
-      <c r="P9" t="str">
-        <v/>
-      </c>
-      <c r="Q9" t="str">
+      <c r="R9" t="str">
+        <v/>
+      </c>
+      <c r="S9" t="str">
         <v>2900</v>
       </c>
-      <c r="R9" t="str">
-        <v>yes</v>
-      </c>
-      <c r="S9" t="str">
+      <c r="T9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="U9" t="str">
         <v>complete</v>
       </c>
-      <c r="T9" t="str">
+      <c r="V9" t="str">
         <v>45755</v>
       </c>
-      <c r="U9" t="str">
+      <c r="W9" t="str">
         <v>in-patient hospice</v>
       </c>
-      <c r="V9" t="str">
+      <c r="X9" t="str">
         <v>3</v>
       </c>
-      <c r="W9" t="str">
+      <c r="Y9" t="str">
         <v>90</v>
       </c>
-      <c r="X9" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y9" t="str">
+      <c r="Z9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA9" t="str">
         <v>no</v>
       </c>
-      <c r="Z9" t="str">
+      <c r="AB9" t="str">
         <v>45760</v>
       </c>
-      <c r="AA9" t="str">
-        <v/>
-      </c>
-      <c r="AB9" t="str">
-        <v/>
-      </c>
       <c r="AC9" t="str">
         <v/>
       </c>
@@ -1280,6 +1330,12 @@
         <v/>
       </c>
       <c r="AF9" t="str">
+        <v/>
+      </c>
+      <c r="AG9" t="str">
+        <v/>
+      </c>
+      <c r="AH9" t="str">
         <v>Eternal Peace</v>
       </c>
     </row>
@@ -1303,71 +1359,71 @@
         <v>Vista</v>
       </c>
       <c r="G10" t="str">
+        <v>951-989-9017</v>
+      </c>
+      <c r="H10" t="str">
+        <v>karen_ingram@gmail.com</v>
+      </c>
+      <c r="I10" t="str">
         <v>45752</v>
       </c>
-      <c r="H10" t="str">
+      <c r="J10" t="str">
         <v>45754</v>
       </c>
-      <c r="I10" t="str">
+      <c r="K10" t="str">
         <v>Dr. Rachel James</v>
       </c>
-      <c r="J10" t="str">
+      <c r="L10" t="str">
         <v>45756</v>
       </c>
-      <c r="K10" t="str">
+      <c r="M10" t="str">
         <v>complete</v>
       </c>
-      <c r="L10" t="str">
+      <c r="N10" t="str">
         <v>45753</v>
       </c>
-      <c r="M10" t="str">
-        <v>yes</v>
-      </c>
-      <c r="N10" t="str">
+      <c r="O10" t="str">
+        <v>yes</v>
+      </c>
+      <c r="P10" t="str">
         <v>Tranquil Care</v>
       </c>
-      <c r="O10" t="str">
+      <c r="Q10" t="str">
         <v>45757</v>
       </c>
-      <c r="P10" t="str">
-        <v/>
-      </c>
-      <c r="Q10" t="str">
+      <c r="R10" t="str">
+        <v/>
+      </c>
+      <c r="S10" t="str">
         <v>4500</v>
       </c>
-      <c r="R10" t="str">
-        <v>yes</v>
-      </c>
-      <c r="S10" t="str">
+      <c r="T10" t="str">
+        <v>yes</v>
+      </c>
+      <c r="U10" t="str">
         <v>complete</v>
       </c>
-      <c r="T10" t="str">
+      <c r="V10" t="str">
         <v>45760</v>
       </c>
-      <c r="U10" t="str">
+      <c r="W10" t="str">
         <v>other</v>
       </c>
-      <c r="V10" t="str">
+      <c r="X10" t="str">
         <v>1</v>
       </c>
-      <c r="W10" t="str">
+      <c r="Y10" t="str">
         <v>20</v>
       </c>
-      <c r="X10" t="str">
+      <c r="Z10" t="str">
         <v>no</v>
       </c>
-      <c r="Y10" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Z10" t="str">
+      <c r="AA10" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB10" t="str">
         <v>45765</v>
       </c>
-      <c r="AA10" t="str">
-        <v/>
-      </c>
-      <c r="AB10" t="str">
-        <v/>
-      </c>
       <c r="AC10" t="str">
         <v/>
       </c>
@@ -1378,6 +1434,12 @@
         <v/>
       </c>
       <c r="AF10" t="str">
+        <v/>
+      </c>
+      <c r="AG10" t="str">
+        <v/>
+      </c>
+      <c r="AH10" t="str">
         <v>Tranquil Care</v>
       </c>
     </row>
@@ -1401,71 +1463,71 @@
         <v>Escondido</v>
       </c>
       <c r="G11" t="str">
+        <v>213-230-2901</v>
+      </c>
+      <c r="H11" t="str">
+        <v>ljackson@hotmail.com</v>
+      </c>
+      <c r="I11" t="str">
         <v>45757</v>
       </c>
-      <c r="H11" t="str">
+      <c r="J11" t="str">
         <v>45759</v>
       </c>
-      <c r="I11" t="str">
+      <c r="K11" t="str">
         <v>Dr. Sam Kline</v>
       </c>
-      <c r="J11" t="str">
+      <c r="L11" t="str">
         <v>45761</v>
       </c>
-      <c r="K11" t="str">
+      <c r="M11" t="str">
         <v>pending</v>
       </c>
-      <c r="L11" t="str">
+      <c r="N11" t="str">
         <v>45758</v>
       </c>
-      <c r="M11" t="str">
+      <c r="O11" t="str">
         <v>no</v>
       </c>
-      <c r="N11" t="str">
+      <c r="P11" t="str">
         <v>Peaceful End</v>
       </c>
-      <c r="O11" t="str">
+      <c r="Q11" t="str">
         <v>45762</v>
       </c>
-      <c r="P11" t="str">
-        <v/>
-      </c>
-      <c r="Q11" t="str">
+      <c r="R11" t="str">
+        <v/>
+      </c>
+      <c r="S11" t="str">
         <v>3100</v>
       </c>
-      <c r="R11" t="str">
+      <c r="T11" t="str">
         <v>no</v>
       </c>
-      <c r="S11" t="str">
+      <c r="U11" t="str">
         <v>in progress</v>
       </c>
-      <c r="T11" t="str">
+      <c r="V11" t="str">
         <v>45765</v>
       </c>
-      <c r="U11" t="str">
+      <c r="W11" t="str">
         <v>private home</v>
       </c>
-      <c r="V11" t="str">
+      <c r="X11" t="str">
         <v>6</v>
       </c>
-      <c r="W11" t="str">
+      <c r="Y11" t="str">
         <v>75</v>
       </c>
-      <c r="X11" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Y11" t="str">
-        <v>yes</v>
-      </c>
       <c r="Z11" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AA11" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AB11" t="str">
         <v>45770</v>
       </c>
-      <c r="AA11" t="str">
-        <v/>
-      </c>
-      <c r="AB11" t="str">
-        <v/>
-      </c>
       <c r="AC11" t="str">
         <v/>
       </c>
@@ -1476,12 +1538,18 @@
         <v/>
       </c>
       <c r="AF11" t="str">
+        <v/>
+      </c>
+      <c r="AG11" t="str">
+        <v/>
+      </c>
+      <c r="AH11" t="str">
         <v>Peaceful End</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AF11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AH11"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1490,7 +1558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -1823,7 +1891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -2057,7 +2125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -3096,9 +3164,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE11"/>
+  <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -3118,71 +3186,71 @@
         <v>Area</v>
       </c>
       <c r="F1" t="str">
+        <v>Phone Number</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="H1" t="str">
         <v>1st request</v>
       </c>
-      <c r="G1" t="str">
+      <c r="I1" t="str">
         <v>2nd request</v>
       </c>
-      <c r="H1" t="str">
+      <c r="J1" t="str">
         <v>CP Doctor</v>
       </c>
-      <c r="I1" t="str">
+      <c r="K1" t="str">
         <v>CP Completed</v>
       </c>
-      <c r="J1" t="str">
+      <c r="L1" t="str">
         <v>RXNT Info</v>
       </c>
-      <c r="K1" t="str">
+      <c r="M1" t="str">
         <v>WR</v>
       </c>
-      <c r="L1" t="str">
+      <c r="N1" t="str">
         <v>Hospice</v>
       </c>
-      <c r="M1" t="str">
+      <c r="O1" t="str">
         <v>Prescription Submit</v>
       </c>
-      <c r="N1" t="str">
-        <v/>
-      </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
+        <v/>
+      </c>
+      <c r="Q1" t="str">
         <v>invoice amount</v>
       </c>
-      <c r="P1" t="str">
+      <c r="R1" t="str">
         <v>PAID</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="S1" t="str">
         <v>Check list</v>
       </c>
-      <c r="R1" t="str">
+      <c r="T1" t="str">
         <v>Ingestion Date</v>
       </c>
-      <c r="S1" t="str">
+      <c r="U1" t="str">
         <v>Ingestion Location</v>
       </c>
-      <c r="T1" t="str">
+      <c r="V1" t="str">
         <v>TTS (Minutes)</v>
       </c>
-      <c r="U1" t="str">
+      <c r="W1" t="str">
         <v>TTD (Minutes)</v>
       </c>
-      <c r="V1" t="str">
+      <c r="X1" t="str">
         <v>Consent Received</v>
       </c>
-      <c r="W1" t="str">
+      <c r="Y1" t="str">
         <v>Medical Records</v>
       </c>
-      <c r="X1" t="str">
+      <c r="Z1" t="str">
         <v>Physician follow up form</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="AA1" t="str">
         <v>EOLOA State</v>
       </c>
-      <c r="Z1" t="str">
-        <v/>
-      </c>
-      <c r="AA1" t="str">
-        <v/>
-      </c>
       <c r="AB1" t="str">
         <v/>
       </c>
@@ -3190,6 +3258,12 @@
         <v/>
       </c>
       <c r="AD1" t="str">
+        <v/>
+      </c>
+      <c r="AE1" t="str">
+        <v/>
+      </c>
+      <c r="AF1" t="str">
         <v>Referred From</v>
       </c>
     </row>
@@ -3210,50 +3284,50 @@
         <v>45231</v>
       </c>
       <c r="F2" t="str">
+        <v>442-450-8177</v>
+      </c>
+      <c r="G2" t="str">
+        <v>phil.spektor@yahoo.com</v>
+      </c>
+      <c r="H2" t="str">
         <v>45261</v>
       </c>
-      <c r="G2" t="str">
+      <c r="I2" t="str">
         <v>Dr. karl Steinber</v>
       </c>
-      <c r="H2" t="str">
+      <c r="J2" t="str">
         <v>45505</v>
       </c>
-      <c r="I2" t="str">
+      <c r="K2" t="str">
         <v>45550</v>
       </c>
-      <c r="J2" t="str">
-        <v>yes</v>
-      </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
+        <v>yes</v>
+      </c>
+      <c r="M2" t="str">
         <v>44928</v>
       </c>
-      <c r="L2" t="str">
-        <v/>
-      </c>
-      <c r="M2" t="str">
+      <c r="N2" t="str">
+        <v/>
+      </c>
+      <c r="O2" t="str">
         <v>45271</v>
       </c>
-      <c r="N2" t="str">
-        <v/>
-      </c>
-      <c r="O2" t="str">
+      <c r="P2" t="str">
+        <v/>
+      </c>
+      <c r="Q2" t="str">
         <v>4125</v>
       </c>
-      <c r="P2" t="str">
-        <v>yes</v>
-      </c>
-      <c r="Q2" t="str">
-        <v/>
-      </c>
       <c r="R2" t="str">
+        <v>yes</v>
+      </c>
+      <c r="S2" t="str">
+        <v/>
+      </c>
+      <c r="T2" t="str">
         <v>private home</v>
       </c>
-      <c r="S2" t="str">
-        <v/>
-      </c>
-      <c r="T2" t="str">
-        <v/>
-      </c>
       <c r="U2" t="str">
         <v/>
       </c>
@@ -3282,6 +3356,12 @@
         <v/>
       </c>
       <c r="AD2" t="str">
+        <v/>
+      </c>
+      <c r="AE2" t="str">
+        <v/>
+      </c>
+      <c r="AF2" t="str">
         <v/>
       </c>
     </row>
@@ -3305,22 +3385,22 @@
         <v/>
       </c>
       <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <v/>
+      </c>
+      <c r="I3" t="str">
         <v>Dr. Susan Bodtkiski</v>
       </c>
-      <c r="H3" t="str">
+      <c r="J3" t="str">
         <v>45518</v>
       </c>
-      <c r="I3" t="str">
+      <c r="K3" t="str">
         <v>45263</v>
       </c>
-      <c r="J3" t="str">
-        <v>yes</v>
-      </c>
-      <c r="K3" t="str">
-        <v/>
-      </c>
       <c r="L3" t="str">
-        <v/>
+        <v>yes</v>
       </c>
       <c r="M3" t="str">
         <v/>
@@ -3353,17 +3433,17 @@
         <v/>
       </c>
       <c r="W3" t="str">
-        <v>yes</v>
+        <v/>
       </c>
       <c r="X3" t="str">
+        <v/>
+      </c>
+      <c r="Y3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="Z3" t="str">
         <v>45160</v>
       </c>
-      <c r="Y3" t="str">
-        <v/>
-      </c>
-      <c r="Z3" t="str">
-        <v/>
-      </c>
       <c r="AA3" t="str">
         <v/>
       </c>
@@ -3374,6 +3454,12 @@
         <v/>
       </c>
       <c r="AD3" t="str">
+        <v/>
+      </c>
+      <c r="AE3" t="str">
+        <v/>
+      </c>
+      <c r="AF3" t="str">
         <v/>
       </c>
     </row>
@@ -3394,53 +3480,53 @@
         <v>San Diego</v>
       </c>
       <c r="F4" t="str">
+        <v>213-321-8235</v>
+      </c>
+      <c r="G4" t="str">
+        <v>rquinn@aol.com</v>
+      </c>
+      <c r="H4" t="str">
         <v>45722</v>
       </c>
-      <c r="G4" t="str">
+      <c r="I4" t="str">
         <v>45724</v>
       </c>
-      <c r="H4" t="str">
+      <c r="J4" t="str">
         <v>Dr. Lisa Green</v>
       </c>
-      <c r="I4" t="str">
+      <c r="K4" t="str">
         <v>45726</v>
       </c>
-      <c r="J4" t="str">
+      <c r="L4" t="str">
         <v>pending</v>
       </c>
-      <c r="K4" t="str">
+      <c r="M4" t="str">
         <v>45723</v>
       </c>
-      <c r="L4" t="str">
-        <v>yes</v>
-      </c>
-      <c r="M4" t="str">
+      <c r="N4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="O4" t="str">
         <v>Radiant</v>
       </c>
-      <c r="N4" t="str">
+      <c r="P4" t="str">
         <v>45727</v>
       </c>
-      <c r="O4" t="str">
-        <v/>
-      </c>
-      <c r="P4" t="str">
+      <c r="Q4" t="str">
+        <v/>
+      </c>
+      <c r="R4" t="str">
         <v>3700</v>
       </c>
-      <c r="Q4" t="str">
+      <c r="S4" t="str">
         <v>no</v>
       </c>
-      <c r="R4" t="str">
+      <c r="T4" t="str">
         <v>in progress</v>
       </c>
-      <c r="S4" t="str">
+      <c r="U4" t="str">
         <v>private home</v>
       </c>
-      <c r="T4" t="str">
-        <v/>
-      </c>
-      <c r="U4" t="str">
-        <v/>
-      </c>
       <c r="V4" t="str">
         <v/>
       </c>
@@ -3469,6 +3555,12 @@
         <v/>
       </c>
       <c r="AE4" t="str">
+        <v/>
+      </c>
+      <c r="AF4" t="str">
+        <v/>
+      </c>
+      <c r="AG4" t="str">
         <v>Radiant Hospice</v>
       </c>
     </row>
@@ -3489,53 +3581,53 @@
         <v>La Jolla</v>
       </c>
       <c r="F5" t="str">
+        <v>323-183-7928</v>
+      </c>
+      <c r="G5" t="str">
+        <v>steve921@outlook.com</v>
+      </c>
+      <c r="H5" t="str">
         <v>45727</v>
       </c>
-      <c r="G5" t="str">
+      <c r="I5" t="str">
         <v>45729</v>
       </c>
-      <c r="H5" t="str">
+      <c r="J5" t="str">
         <v>Dr. Mark Hale</v>
       </c>
-      <c r="I5" t="str">
+      <c r="K5" t="str">
         <v>45731</v>
       </c>
-      <c r="J5" t="str">
+      <c r="L5" t="str">
         <v>pending</v>
       </c>
-      <c r="K5" t="str">
+      <c r="M5" t="str">
         <v>45728</v>
       </c>
-      <c r="L5" t="str">
+      <c r="N5" t="str">
         <v>no</v>
       </c>
-      <c r="M5" t="str">
+      <c r="O5" t="str">
         <v>Serenity Hospice</v>
       </c>
-      <c r="N5" t="str">
+      <c r="P5" t="str">
         <v>45732</v>
       </c>
-      <c r="O5" t="str">
-        <v/>
-      </c>
-      <c r="P5" t="str">
+      <c r="Q5" t="str">
+        <v/>
+      </c>
+      <c r="R5" t="str">
         <v>3000</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="S5" t="str">
         <v>no</v>
       </c>
-      <c r="R5" t="str">
+      <c r="T5" t="str">
         <v>in progress</v>
       </c>
-      <c r="S5" t="str">
+      <c r="U5" t="str">
         <v>assisted living</v>
       </c>
-      <c r="T5" t="str">
-        <v/>
-      </c>
-      <c r="U5" t="str">
-        <v/>
-      </c>
       <c r="V5" t="str">
         <v/>
       </c>
@@ -3564,6 +3656,12 @@
         <v/>
       </c>
       <c r="AE5" t="str">
+        <v/>
+      </c>
+      <c r="AF5" t="str">
+        <v/>
+      </c>
+      <c r="AG5" t="str">
         <v>Serenity Hospice</v>
       </c>
     </row>
@@ -3584,53 +3682,53 @@
         <v>Encinitas</v>
       </c>
       <c r="F6" t="str">
+        <v>442-709-5063</v>
+      </c>
+      <c r="G6" t="str">
+        <v>tina.santos@hotmail.com</v>
+      </c>
+      <c r="H6" t="str">
         <v>45732</v>
       </c>
-      <c r="G6" t="str">
+      <c r="I6" t="str">
         <v>45734</v>
       </c>
-      <c r="H6" t="str">
+      <c r="J6" t="str">
         <v>Dr. Nina Ford</v>
       </c>
-      <c r="I6" t="str">
+      <c r="K6" t="str">
         <v>45736</v>
       </c>
-      <c r="J6" t="str">
+      <c r="L6" t="str">
         <v>pending</v>
       </c>
-      <c r="K6" t="str">
+      <c r="M6" t="str">
         <v>45733</v>
       </c>
-      <c r="L6" t="str">
-        <v>yes</v>
-      </c>
-      <c r="M6" t="str">
+      <c r="N6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="O6" t="str">
         <v>Harmony Care</v>
       </c>
-      <c r="N6" t="str">
+      <c r="P6" t="str">
         <v>45737</v>
       </c>
-      <c r="O6" t="str">
-        <v/>
-      </c>
-      <c r="P6" t="str">
+      <c r="Q6" t="str">
+        <v/>
+      </c>
+      <c r="R6" t="str">
         <v>4000</v>
       </c>
-      <c r="Q6" t="str">
+      <c r="S6" t="str">
         <v>no</v>
       </c>
-      <c r="R6" t="str">
+      <c r="T6" t="str">
         <v>in progress</v>
       </c>
-      <c r="S6" t="str">
+      <c r="U6" t="str">
         <v>acute care hospital</v>
       </c>
-      <c r="T6" t="str">
-        <v/>
-      </c>
-      <c r="U6" t="str">
-        <v/>
-      </c>
       <c r="V6" t="str">
         <v/>
       </c>
@@ -3659,6 +3757,12 @@
         <v/>
       </c>
       <c r="AE6" t="str">
+        <v/>
+      </c>
+      <c r="AF6" t="str">
+        <v/>
+      </c>
+      <c r="AG6" t="str">
         <v>Harmony Care</v>
       </c>
     </row>
@@ -3679,53 +3783,53 @@
         <v>Oceanside</v>
       </c>
       <c r="F7" t="str">
+        <v>760-335-2451</v>
+      </c>
+      <c r="G7" t="str">
+        <v>utorres@gmail.com</v>
+      </c>
+      <c r="H7" t="str">
         <v>45737</v>
       </c>
-      <c r="G7" t="str">
+      <c r="I7" t="str">
         <v>45739</v>
       </c>
-      <c r="H7" t="str">
+      <c r="J7" t="str">
         <v>Dr. Owen Gray</v>
       </c>
-      <c r="I7" t="str">
+      <c r="K7" t="str">
         <v>45741</v>
       </c>
-      <c r="J7" t="str">
+      <c r="L7" t="str">
         <v>pending</v>
       </c>
-      <c r="K7" t="str">
+      <c r="M7" t="str">
         <v>45738</v>
       </c>
-      <c r="L7" t="str">
+      <c r="N7" t="str">
         <v>no</v>
       </c>
-      <c r="M7" t="str">
+      <c r="O7" t="str">
         <v>Coastal Hospice</v>
       </c>
-      <c r="N7" t="str">
+      <c r="P7" t="str">
         <v>45742</v>
       </c>
-      <c r="O7" t="str">
-        <v/>
-      </c>
-      <c r="P7" t="str">
+      <c r="Q7" t="str">
+        <v/>
+      </c>
+      <c r="R7" t="str">
         <v>3200</v>
       </c>
-      <c r="Q7" t="str">
+      <c r="S7" t="str">
         <v>no</v>
       </c>
-      <c r="R7" t="str">
+      <c r="T7" t="str">
         <v>in progress</v>
       </c>
-      <c r="S7" t="str">
+      <c r="U7" t="str">
         <v>in-patient hospice</v>
       </c>
-      <c r="T7" t="str">
-        <v/>
-      </c>
-      <c r="U7" t="str">
-        <v/>
-      </c>
       <c r="V7" t="str">
         <v/>
       </c>
@@ -3754,6 +3858,12 @@
         <v/>
       </c>
       <c r="AE7" t="str">
+        <v/>
+      </c>
+      <c r="AF7" t="str">
+        <v/>
+      </c>
+      <c r="AG7" t="str">
         <v>Coastal Hospice</v>
       </c>
     </row>
@@ -3774,53 +3884,53 @@
         <v>Carlsbad</v>
       </c>
       <c r="F8" t="str">
+        <v>619-317-1799</v>
+      </c>
+      <c r="G8" t="str">
+        <v>victoria_underwood@aol.com</v>
+      </c>
+      <c r="H8" t="str">
         <v>45742</v>
       </c>
-      <c r="G8" t="str">
+      <c r="I8" t="str">
         <v>45744</v>
       </c>
-      <c r="H8" t="str">
+      <c r="J8" t="str">
         <v>Dr. Paula Hunt</v>
       </c>
-      <c r="I8" t="str">
+      <c r="K8" t="str">
         <v>45746</v>
       </c>
-      <c r="J8" t="str">
+      <c r="L8" t="str">
         <v>pending</v>
       </c>
-      <c r="K8" t="str">
+      <c r="M8" t="str">
         <v>45743</v>
       </c>
-      <c r="L8" t="str">
-        <v>yes</v>
-      </c>
-      <c r="M8" t="str">
+      <c r="N8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="O8" t="str">
         <v>Sunrise Hospice</v>
       </c>
-      <c r="N8" t="str">
+      <c r="P8" t="str">
         <v>45747</v>
       </c>
-      <c r="O8" t="str">
-        <v/>
-      </c>
-      <c r="P8" t="str">
+      <c r="Q8" t="str">
+        <v/>
+      </c>
+      <c r="R8" t="str">
         <v>3900</v>
       </c>
-      <c r="Q8" t="str">
+      <c r="S8" t="str">
         <v>no</v>
       </c>
-      <c r="R8" t="str">
+      <c r="T8" t="str">
         <v>in progress</v>
       </c>
-      <c r="S8" t="str">
+      <c r="U8" t="str">
         <v>other</v>
       </c>
-      <c r="T8" t="str">
-        <v/>
-      </c>
-      <c r="U8" t="str">
-        <v/>
-      </c>
       <c r="V8" t="str">
         <v/>
       </c>
@@ -3849,6 +3959,12 @@
         <v/>
       </c>
       <c r="AE8" t="str">
+        <v/>
+      </c>
+      <c r="AF8" t="str">
+        <v/>
+      </c>
+      <c r="AG8" t="str">
         <v>Sunrise Hospice</v>
       </c>
     </row>
@@ -3869,53 +3985,53 @@
         <v>Del Mar</v>
       </c>
       <c r="F9" t="str">
+        <v>562-211-7829</v>
+      </c>
+      <c r="G9" t="str">
+        <v>williamvargas@outlook.com</v>
+      </c>
+      <c r="H9" t="str">
         <v>45747</v>
       </c>
-      <c r="G9" t="str">
+      <c r="I9" t="str">
         <v>45749</v>
       </c>
-      <c r="H9" t="str">
+      <c r="J9" t="str">
         <v>Dr. Quentin Ives</v>
       </c>
-      <c r="I9" t="str">
+      <c r="K9" t="str">
         <v>45751</v>
       </c>
-      <c r="J9" t="str">
+      <c r="L9" t="str">
         <v>pending</v>
       </c>
-      <c r="K9" t="str">
+      <c r="M9" t="str">
         <v>45748</v>
       </c>
-      <c r="L9" t="str">
+      <c r="N9" t="str">
         <v>no</v>
       </c>
-      <c r="M9" t="str">
+      <c r="O9" t="str">
         <v>Eternal Peace</v>
       </c>
-      <c r="N9" t="str">
+      <c r="P9" t="str">
         <v>45752</v>
       </c>
-      <c r="O9" t="str">
-        <v/>
-      </c>
-      <c r="P9" t="str">
+      <c r="Q9" t="str">
+        <v/>
+      </c>
+      <c r="R9" t="str">
         <v>4300</v>
       </c>
-      <c r="Q9" t="str">
+      <c r="S9" t="str">
         <v>no</v>
       </c>
-      <c r="R9" t="str">
+      <c r="T9" t="str">
         <v>in progress</v>
       </c>
-      <c r="S9" t="str">
+      <c r="U9" t="str">
         <v>private home</v>
       </c>
-      <c r="T9" t="str">
-        <v/>
-      </c>
-      <c r="U9" t="str">
-        <v/>
-      </c>
       <c r="V9" t="str">
         <v/>
       </c>
@@ -3944,6 +4060,12 @@
         <v/>
       </c>
       <c r="AE9" t="str">
+        <v/>
+      </c>
+      <c r="AF9" t="str">
+        <v/>
+      </c>
+      <c r="AG9" t="str">
         <v>Eternal Peace</v>
       </c>
     </row>
@@ -3964,53 +4086,53 @@
         <v>Vista</v>
       </c>
       <c r="F10" t="str">
+        <v>619-367-4098</v>
+      </c>
+      <c r="G10" t="str">
+        <v>xena.valdez@hotmail.com</v>
+      </c>
+      <c r="H10" t="str">
         <v>45752</v>
       </c>
-      <c r="G10" t="str">
+      <c r="I10" t="str">
         <v>45754</v>
       </c>
-      <c r="H10" t="str">
+      <c r="J10" t="str">
         <v>Dr. Rachel James</v>
       </c>
-      <c r="I10" t="str">
+      <c r="K10" t="str">
         <v>45756</v>
       </c>
-      <c r="J10" t="str">
+      <c r="L10" t="str">
         <v>pending</v>
       </c>
-      <c r="K10" t="str">
+      <c r="M10" t="str">
         <v>45753</v>
       </c>
-      <c r="L10" t="str">
-        <v>yes</v>
-      </c>
-      <c r="M10" t="str">
+      <c r="N10" t="str">
+        <v>yes</v>
+      </c>
+      <c r="O10" t="str">
         <v>Tranquil Care</v>
       </c>
-      <c r="N10" t="str">
+      <c r="P10" t="str">
         <v>45757</v>
       </c>
-      <c r="O10" t="str">
-        <v/>
-      </c>
-      <c r="P10" t="str">
+      <c r="Q10" t="str">
+        <v/>
+      </c>
+      <c r="R10" t="str">
         <v>3400</v>
       </c>
-      <c r="Q10" t="str">
+      <c r="S10" t="str">
         <v>no</v>
       </c>
-      <c r="R10" t="str">
+      <c r="T10" t="str">
         <v>in progress</v>
       </c>
-      <c r="S10" t="str">
+      <c r="U10" t="str">
         <v>assisted living</v>
       </c>
-      <c r="T10" t="str">
-        <v/>
-      </c>
-      <c r="U10" t="str">
-        <v/>
-      </c>
       <c r="V10" t="str">
         <v/>
       </c>
@@ -4039,6 +4161,12 @@
         <v/>
       </c>
       <c r="AE10" t="str">
+        <v/>
+      </c>
+      <c r="AF10" t="str">
+        <v/>
+      </c>
+      <c r="AG10" t="str">
         <v>Tranquil Care</v>
       </c>
     </row>
@@ -4059,53 +4187,53 @@
         <v>Escondido</v>
       </c>
       <c r="F11" t="str">
+        <v>760-710-6342</v>
+      </c>
+      <c r="G11" t="str">
+        <v>yosef.vasquez@hotmail.com</v>
+      </c>
+      <c r="H11" t="str">
         <v>45757</v>
       </c>
-      <c r="G11" t="str">
+      <c r="I11" t="str">
         <v>45759</v>
       </c>
-      <c r="H11" t="str">
+      <c r="J11" t="str">
         <v>Dr. Sam Kline</v>
       </c>
-      <c r="I11" t="str">
+      <c r="K11" t="str">
         <v>45761</v>
       </c>
-      <c r="J11" t="str">
+      <c r="L11" t="str">
         <v>pending</v>
       </c>
-      <c r="K11" t="str">
+      <c r="M11" t="str">
         <v>45758</v>
       </c>
-      <c r="L11" t="str">
+      <c r="N11" t="str">
         <v>no</v>
       </c>
-      <c r="M11" t="str">
+      <c r="O11" t="str">
         <v>Peaceful End</v>
       </c>
-      <c r="N11" t="str">
+      <c r="P11" t="str">
         <v>45762</v>
       </c>
-      <c r="O11" t="str">
-        <v/>
-      </c>
-      <c r="P11" t="str">
+      <c r="Q11" t="str">
+        <v/>
+      </c>
+      <c r="R11" t="str">
         <v>4100</v>
       </c>
-      <c r="Q11" t="str">
+      <c r="S11" t="str">
         <v>no</v>
       </c>
-      <c r="R11" t="str">
+      <c r="T11" t="str">
         <v>in progress</v>
       </c>
-      <c r="S11" t="str">
+      <c r="U11" t="str">
         <v>acute care hospital</v>
       </c>
-      <c r="T11" t="str">
-        <v/>
-      </c>
-      <c r="U11" t="str">
-        <v/>
-      </c>
       <c r="V11" t="str">
         <v/>
       </c>
@@ -4134,12 +4262,18 @@
         <v/>
       </c>
       <c r="AE11" t="str">
+        <v/>
+      </c>
+      <c r="AF11" t="str">
+        <v/>
+      </c>
+      <c r="AG11" t="str">
         <v>Peaceful End</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AG11"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -4148,7 +4282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -4475,4 +4609,661 @@
     <ignoredError numberStoredAsText="1" sqref="A1:I11"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Vendor ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Company Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Category</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Service Type</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Contact Person</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Address</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Website</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Notes</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Rating</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Last Contact</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Status</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>V001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Serenity Cremation Services</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Cremation</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Cremation &amp; Memorial</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Sarah Johnson</v>
+      </c>
+      <c r="F2" t="str">
+        <v>(555) 123-4567</v>
+      </c>
+      <c r="G2" t="str">
+        <v>sarah@serenitycremation.com</v>
+      </c>
+      <c r="H2" t="str">
+        <v>123 Peaceful Lane, Riverside, CA 92501</v>
+      </c>
+      <c r="I2" t="str">
+        <v>www.serenitycremation.com</v>
+      </c>
+      <c r="J2" t="str">
+        <v>Reliable service, good pricing</v>
+      </c>
+      <c r="K2" t="str">
+        <v>4.8</v>
+      </c>
+      <c r="L2" t="str">
+        <v>2024-01-15</v>
+      </c>
+      <c r="M2" t="str">
+        <v>Active</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>V002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Compassionate Care Pharmacies</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Pharmacy</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Hospice Medications</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Dr. Michael Chen</v>
+      </c>
+      <c r="F3" t="str">
+        <v>(555) 234-5678</v>
+      </c>
+      <c r="G3" t="str">
+        <v>mchen@compcarepharm.com</v>
+      </c>
+      <c r="H3" t="str">
+        <v>456 Medical Plaza, Riverside, CA 92503</v>
+      </c>
+      <c r="I3" t="str">
+        <v>www.compcarepharm.com</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Specializes in pain management meds</v>
+      </c>
+      <c r="K3" t="str">
+        <v>4.9</v>
+      </c>
+      <c r="L3" t="str">
+        <v>2024-01-20</v>
+      </c>
+      <c r="M3" t="str">
+        <v>Active</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>V003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Gentle Hands Doula Services</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Doula</v>
+      </c>
+      <c r="D4" t="str">
+        <v>End-of-Life Support</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Maria Rodriguez</v>
+      </c>
+      <c r="F4" t="str">
+        <v>(555) 345-6789</v>
+      </c>
+      <c r="G4" t="str">
+        <v>maria@gentlehands.com</v>
+      </c>
+      <c r="H4" t="str">
+        <v>789 Comfort Way, Riverside, CA 92505</v>
+      </c>
+      <c r="I4" t="str">
+        <v>www.gentlehands.com</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Excellent bedside manner, 24/7 availability</v>
+      </c>
+      <c r="K4" t="str">
+        <v>5.0</v>
+      </c>
+      <c r="L4" t="str">
+        <v>2024-01-18</v>
+      </c>
+      <c r="M4" t="str">
+        <v>Active</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>V004</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Eternal Rest Funeral Home</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Funeral Services</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Funeral &amp; Memorial</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Robert Williams</v>
+      </c>
+      <c r="F5" t="str">
+        <v>(555) 456-7890</v>
+      </c>
+      <c r="G5" t="str">
+        <v>rwilliams@eternalrest.com</v>
+      </c>
+      <c r="H5" t="str">
+        <v>321 Memorial Drive, Riverside, CA 92507</v>
+      </c>
+      <c r="I5" t="str">
+        <v>www.eternalrest.com</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Traditional services, family-owned</v>
+      </c>
+      <c r="K5" t="str">
+        <v>4.7</v>
+      </c>
+      <c r="L5" t="str">
+        <v>2024-01-12</v>
+      </c>
+      <c r="M5" t="str">
+        <v>Active</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>V005</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Hospice Equipment Supply Co.</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Medical Equipment</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Durable Medical Equipment</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Jennifer Davis</v>
+      </c>
+      <c r="F6" t="str">
+        <v>(555) 567-8901</v>
+      </c>
+      <c r="G6" t="str">
+        <v>jdavis@hospiceequipment.com</v>
+      </c>
+      <c r="H6" t="str">
+        <v>654 Medical Supply Blvd, Riverside, CA 92509</v>
+      </c>
+      <c r="I6" t="str">
+        <v>www.hospiceequipment.com</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Quick delivery, wide selection</v>
+      </c>
+      <c r="K6" t="str">
+        <v>4.6</v>
+      </c>
+      <c r="L6" t="str">
+        <v>2024-01-22</v>
+      </c>
+      <c r="M6" t="str">
+        <v>Active</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>V006</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Peaceful Transitions Counseling</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Counseling</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Grief &amp; Bereavement</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Dr. Lisa Thompson</v>
+      </c>
+      <c r="F7" t="str">
+        <v>(555) 678-9012</v>
+      </c>
+      <c r="G7" t="str">
+        <v>lthompson@peacefultransitions.com</v>
+      </c>
+      <c r="H7" t="str">
+        <v>987 Healing Circle, Riverside, CA 92511</v>
+      </c>
+      <c r="I7" t="str">
+        <v>www.peacefultransitions.com</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Licensed therapists, sliding scale fees</v>
+      </c>
+      <c r="K7" t="str">
+        <v>4.9</v>
+      </c>
+      <c r="L7" t="str">
+        <v>2024-01-16</v>
+      </c>
+      <c r="M7" t="str">
+        <v>Active</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:M7"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Timestamp</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Type</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Participants</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Sender</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Message</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Tags</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>20241201143000</v>
+      </c>
+      <c r="B2" t="str">
+        <v>GM</v>
+      </c>
+      <c r="C2" t="str">
+        <v>&lt;Alyssa&gt;&lt;Dr. Moore&gt;&lt;Christa&gt;&lt;Amber&gt;</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Alyssa</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Hey team, where are we on the Johnson case?</v>
+      </c>
+      <c r="F2" t="str">
+        <v>active</v>
+      </c>
+      <c r="G2" t="str">
+        <v>patient-update</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>20241201143100</v>
+      </c>
+      <c r="B3" t="str">
+        <v>GM</v>
+      </c>
+      <c r="C3" t="str">
+        <v>&lt;Alyssa&gt;&lt;Dr. Moore&gt;&lt;Christa&gt;&lt;Amber&gt;</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Dr. Moore</v>
+      </c>
+      <c r="E3" t="str">
+        <v>I just reviewed the medication list, all looks good</v>
+      </c>
+      <c r="F3" t="str">
+        <v>active</v>
+      </c>
+      <c r="G3" t="str">
+        <v>medical-review</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>20241201143200</v>
+      </c>
+      <c r="B4" t="str">
+        <v>DM</v>
+      </c>
+      <c r="C4" t="str">
+        <v>&lt;Alyssa&gt;&lt;Christa&gt;</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Christa</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Family meeting scheduled for tomorrow at 2pm</v>
+      </c>
+      <c r="F4" t="str">
+        <v>active</v>
+      </c>
+      <c r="G4" t="str">
+        <v>meeting</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>20241201143300</v>
+      </c>
+      <c r="B5" t="str">
+        <v>DM</v>
+      </c>
+      <c r="C5" t="str">
+        <v>&lt;Alyssa&gt;&lt;Amber&gt;</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Alyssa</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Hey Amber, can you prep the meeting notes?</v>
+      </c>
+      <c r="F5" t="str">
+        <v>active</v>
+      </c>
+      <c r="G5" t="str">
+        <v>task</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>20241201143400</v>
+      </c>
+      <c r="B6" t="str">
+        <v>GM</v>
+      </c>
+      <c r="C6" t="str">
+        <v>&lt;Alyssa&gt;&lt;Dr. Moore&gt;&lt;Christa&gt;&lt;Amber&gt;</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Amber</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Welcome Amber! Please connect with Alyssa on this new project</v>
+      </c>
+      <c r="F6" t="str">
+        <v>active</v>
+      </c>
+      <c r="G6" t="str">
+        <v>onboarding</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>20241201143500</v>
+      </c>
+      <c r="B7" t="str">
+        <v>DM</v>
+      </c>
+      <c r="C7" t="str">
+        <v>&lt;Dr. Moore&gt;&lt;Christa&gt;</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Dr. Moore</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Christa, can you review the Johnson medication schedule?</v>
+      </c>
+      <c r="F7" t="str">
+        <v>active</v>
+      </c>
+      <c r="G7" t="str">
+        <v>medical-task</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>20241201143600</v>
+      </c>
+      <c r="B8" t="str">
+        <v>GM</v>
+      </c>
+      <c r="C8" t="str">
+        <v>&lt;Alyssa&gt;&lt;Dr. Moore&gt;&lt;Christa&gt;&lt;Amber&gt;</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Alyssa</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Insurance approval came through for the Smith family!</v>
+      </c>
+      <c r="F8" t="str">
+        <v>active</v>
+      </c>
+      <c r="G8" t="str">
+        <v>good-news</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>20241201143700</v>
+      </c>
+      <c r="B9" t="str">
+        <v>DM</v>
+      </c>
+      <c r="C9" t="str">
+        <v>&lt;Alyssa&gt;&lt;Donnie&gt;</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Alyssa</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Hey Donnie, lets get Amber onboarded properly</v>
+      </c>
+      <c r="F9" t="str">
+        <v>active</v>
+      </c>
+      <c r="G9" t="str">
+        <v>onboarding</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>20241201143800</v>
+      </c>
+      <c r="B10" t="str">
+        <v>GM</v>
+      </c>
+      <c r="C10" t="str">
+        <v>&lt;Alyssa&gt;&lt;Donnie&gt;&lt;Amber&gt;</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Donnie</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Welcome Amber! Please connect with Alyssa on this new project</v>
+      </c>
+      <c r="F10" t="str">
+        <v>active</v>
+      </c>
+      <c r="G10" t="str">
+        <v>welcome</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>20241201143900</v>
+      </c>
+      <c r="B11" t="str">
+        <v>NOTE</v>
+      </c>
+      <c r="C11" t="str">
+        <v>&lt;Alyssa&gt;</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Alyssa</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Patient timeline updated - family meeting scheduled</v>
+      </c>
+      <c r="F11" t="str">
+        <v>active</v>
+      </c>
+      <c r="G11" t="str">
+        <v>patient-timeline</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>20241201144000</v>
+      </c>
+      <c r="B12" t="str">
+        <v>NOTE</v>
+      </c>
+      <c r="C12" t="str">
+        <v>&lt;Dr. Moore&gt;</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Dr. Moore</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Medication review completed - no changes needed</v>
+      </c>
+      <c r="F12" t="str">
+        <v>active</v>
+      </c>
+      <c r="G12" t="str">
+        <v>medical-note</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>20241201144100</v>
+      </c>
+      <c r="B13" t="str">
+        <v>DM</v>
+      </c>
+      <c r="C13" t="str">
+        <v>&lt;Christa&gt;&lt;Amber&gt;</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Christa</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Amber, here are the key contacts for the Johnson case</v>
+      </c>
+      <c r="F13" t="str">
+        <v>active</v>
+      </c>
+      <c r="G13" t="str">
+        <v>contacts</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>20241201144200</v>
+      </c>
+      <c r="B14" t="str">
+        <v>GM</v>
+      </c>
+      <c r="C14" t="str">
+        <v>&lt;Alyssa&gt;&lt;Dr. Moore&gt;&lt;Christa&gt;&lt;Amber&gt;</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Amber</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Thanks everyone! Excited to be part of the team</v>
+      </c>
+      <c r="F14" t="str">
+        <v>active</v>
+      </c>
+      <c r="G14" t="str">
+        <v>introduction</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>20250803030334</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Alyssa</v>
+      </c>
+      <c r="C15" t="str">
+        <v>test</v>
+      </c>
+      <c r="D15" t="str">
+        <v>GM</v>
+      </c>
+      <c r="E15" t="str">
+        <v>all</v>
+      </c>
+      <c r="F15" t="str">
+        <v>active</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:G15"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>